<commit_message>
update report after final reminder delphi 1
</commit_message>
<xml_diff>
--- a/data/clean/Delphi1.xlsx
+++ b/data/clean/Delphi1.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="271">
   <si>
     <t>StartDate</t>
   </si>
@@ -161,6 +161,30 @@
     <t>20</t>
   </si>
   <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
     <t>IP Address</t>
   </si>
   <si>
@@ -224,6 +248,30 @@
     <t>129.177.198.47</t>
   </si>
   <si>
+    <t>86.160.3.111</t>
+  </si>
+  <si>
+    <t>185.80.79.95</t>
+  </si>
+  <si>
+    <t>86.176.139.85</t>
+  </si>
+  <si>
+    <t>84.208.127.41</t>
+  </si>
+  <si>
+    <t>84.9.85.21</t>
+  </si>
+  <si>
+    <t>62.194.218.41</t>
+  </si>
+  <si>
+    <t>77.174.227.110</t>
+  </si>
+  <si>
+    <t>71.105.254.23</t>
+  </si>
+  <si>
     <t>TRUE</t>
   </si>
   <si>
@@ -287,6 +335,30 @@
     <t>R_41qoVspNApmcL1D</t>
   </si>
   <si>
+    <t>R_24uXMWhE2RHxFqa</t>
+  </si>
+  <si>
+    <t>R_2e7SQSWchlcS4Oh</t>
+  </si>
+  <si>
+    <t>R_1YXqfdYleMGsL11</t>
+  </si>
+  <si>
+    <t>R_6f3JXqXWyGx7Fon</t>
+  </si>
+  <si>
+    <t>R_4KoSJ5c6GoAg1nD</t>
+  </si>
+  <si>
+    <t>R_30TlEs2612tRoHb</t>
+  </si>
+  <si>
+    <t>R_2L6n7tjefCZ1dDb</t>
+  </si>
+  <si>
+    <t>R_77I1BFSeoy3XnH7</t>
+  </si>
+  <si>
     <t>email</t>
   </si>
   <si>
@@ -296,6 +368,9 @@
     <t>Yes</t>
   </si>
   <si>
+    <t>No</t>
+  </si>
+  <si>
     <t>Academic researcher</t>
   </si>
   <si>
@@ -333,9 +408,6 @@
   </si>
   <si>
     <t>Asia</t>
-  </si>
-  <si>
-    <t>No</t>
   </si>
   <si>
     <t>Take care of their own mental health, so that they can remain empathetic.</t>
@@ -469,6 +541,39 @@
 4. Be trained in scalable psychological interventions (ex. PFA, SH+, PM+)</t>
   </si>
   <si>
+    <t xml:space="preserve">1. be aware of the unique cluster of relevant variables that they bring to the work. These include awareness of the impact that 
+(a) their own personal features and background (e.g. ethnic, cultural, religious/spiritual, educational, social status, linguistic, gender, age, etc) would have on the Asylum Seekers (AS)
+(b) their own organisation's relevant features and background would have on the AS (e.g. explicit or implicit ideology, source of funding, history and record of involvement on comparable situations in other contexts, etc);
+2. be aware of the unique cluster of relevant variables of the AS with whom they are conversing (e.g. ethnic, cultural, religious/spiritual, educational, social status, linguistic, gender, age, disability, etc);
+3. be aware of the unique context within which they are conducting such conversations with AS (e.g. as part of a humanitarian assistance effort, or of an evaluation of assistance needs, etc);
+4. Be aware of and practice Cultural Humility. 
+</t>
+  </si>
+  <si>
+    <t>treat asylum applicants first and foremost as human beings with similar struggles, challenges, hopes and dreams as themselves; should have knowledge about the factors impacting refugees' mental health; should be able to challenge their own views and solutions (and stereotypes), and inquire and include the views and solutions of their clients</t>
+  </si>
+  <si>
+    <t>1) be trained and supported in developing a trauma- informed approach
+2) clinical supervision and self care 
+3) trained in a survivor centric approach
+4) cultural competences and concepts relevant to transcultural formulations and interventions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) be able to establish a relationship of trust and empathy;
+2) have basic knowledge of mental health resources (resilience) and reactions to war-related trauma;
+3) have basic knowledge about cultural variations in knowledge and understanding of mental health (problems);
+</t>
+  </si>
+  <si>
+    <t>1. take the lead from asylum seekers; 2. resist racist government policies; 3. adopt a anti-colonial perspective; 4. have cultural humility; 5. be curious.</t>
+  </si>
+  <si>
+    <t>Be aware of esp. all the current stressors</t>
+  </si>
+  <si>
+    <t>I work with immigrants, refugees and asylum seekers. Most of the asylum seekers I have worked with have been in the context of Mental Health evaluation to support asylum claims, psychotherapy with asylum seekers in hospital and community settings, and training of therapists, and immigration officers in cultural and strucural sensitivity.  In these contexts it is important that the front line workers have education and consultation with a knowledgeable representative (preferably professional) of the culture of the asylum seekers with which one is working.  The transcultural conversations ideally should seek to understand the clients perspective and cultural form of describing distress and its sources, as well as preferred ways of addressing that distress. In addition, what individual, social, cultural resources one needs to draw on to promote psychosocial well-being.</t>
+  </si>
+  <si>
     <t>Psychological first aid</t>
   </si>
   <si>
@@ -541,6 +646,30 @@
   </si>
   <si>
     <t>IASC Guidelines on Mental Health and Psychosocial Support in Emergency Settings, 2007</t>
+  </si>
+  <si>
+    <t>The above, plus the 'Adversity Grid' (Papadopoulos, 2004, 2007, 2021), which enables workers to appreciate not only (a) the negative effects of the AS's plight, i.e. the way they were damaged by their adversity (e.g. losses, trauma, etc), but also (b) their retained strengths (which they had acquired before their exposure to adversity) i.e. resilient features, and (c) their new strengths (which they acquired because of their very exposure to adversity), i.e. 'Adversity-Activated Development’.</t>
+  </si>
+  <si>
+    <t>balance between diversity and inclusion, being the same and being different; and looking for continuity in live; contextual theory of Boszormenyi-Nagy</t>
+  </si>
+  <si>
+    <t>1) IASC- MHPSS guidelines
+2) WHO 
+3) the medical anthropology and psychological anthropology literature</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) I recognize that arrival at one of the hot spots or asylum centers in low income countries is very different from arrival in European high income countries with restrictive immigration policies (i.e. low numbers of arrivals). Nevertheless, providing support from a psychosocial first aid framework is important in the first stage;
+</t>
+  </si>
+  <si>
+    <t>I co-developed these guidelines for mental health practitioners working with Afghan sanctuary seekers: https://www.sohailj.com/wp-content/uploads/2022/08/MentalHealthGuide_v4.pdf</t>
+  </si>
+  <si>
+    <t>My own. Approaching culture as a buffer for stress</t>
+  </si>
+  <si>
+    <t>I participated in the development of the IOM Guidelines for Community based Mental Health and Psychosocial Support in Emergency and Migrant situations. That is a very good source.</t>
   </si>
   <si>
     <t>Probably yes</t>
@@ -670,6 +799,37 @@
 </t>
   </si>
   <si>
+    <t>I have identified the main principles above. 
+In terms of knowledge, they should be aware of specific knowledge that helps them appreciate the above and put them into practice.</t>
+  </si>
+  <si>
+    <t>these are human beings with similar hopes, dreams and challenges as all other human beings (including the frontline workers themselves), yet migration also poses particular challenges</t>
+  </si>
+  <si>
+    <t>1) understand local concepts of the mind and healing
+2) advanced in cultural constructions and impact of collective trauma and of extreme violence 
+3) literature around victims and survivors approaches</t>
+  </si>
+  <si>
+    <t>My work has mainly been with unaccompanied asylum-seeking minors, which is important context for the following responses
+1) asylum-seeking children and youth (ASM) are typically struggling with a series of practical problems that they need to solve before they are ready to address their own mental health issues; 
+2) ASM are often silent about their mental health problems as they believe they may impact on their asylum-application;
+3) ASM may be afraid that their mental reactions are a sign that they are turning crazy;  
+4) helping with practical problems and informing ASM about mental health on a general level (education) may be a way to establishing trust and reducing anxiety; 
+5) Identifying and scaffolding the streghts and coping resources of ASM is as important as identifying risk factors and symptoms of mental health problems;</t>
+  </si>
+  <si>
+    <t>1. borders are violent; 2. people are resisting political oppression on a daily basis.</t>
+  </si>
+  <si>
+    <t>Lowering stress improves trust and understanding</t>
+  </si>
+  <si>
+    <t>Asylum seekers may come from societies that do not have developed mental health systems and may equate mental health services with psychiatric treatment of the severely mentally ill.
+To repeat fro, first question, they need to know that asylum seekers may have their own cultural forms of describing distress and mental health issues, and preferred solutions to those problems.
+They need to know how to have conversations that enable both asylum seeker and front line worker to understand individual. social and cultural resources that they see as helpful in addressing psychosocial difficulties and promoting well-being.</t>
+  </si>
+  <si>
     <t>Ask questions to elicit explanatory models and cultural concepts of distress</t>
   </si>
   <si>
@@ -773,6 +933,40 @@
 2. Use concrete tools in their work that can guide their practice. 
 3. Receive supervision and ongoing training that should be culturally adapted to the population they provide help to.
 4. Know the basic legal system and be alert to identify violations of human rights in different levels.</t>
+  </si>
+  <si>
+    <t>I have identified the main principles above. 
+In terms of skills, they should be aware of specific skills that help them appreciate the above and put them into practice. 
+More specifically, they should be able to relate at a human level with AS and not see them as specimens of an exotic 'other' group of people.</t>
+  </si>
+  <si>
+    <t>really listen to the other, and being able to question their own views, experiences, solutions and steoretypes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Same than above in its implementation 
+In addition 
+1) legal skills 
+2) understand local government policies
+3) navigate local services
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) establish a relationship of trust and safety;
+2) normalize mental health reactions to stressful and traumatic events;
+3) conduct the conversation from a strength (resilience) perspective;
+4) observe and identify symptoms of common disorders among ASM;
+5) talk with the ASM in a direct and understandable language;
+</t>
+  </si>
+  <si>
+    <t>1. have empathy and solidarity; 2. take part in a shared struggle.</t>
+  </si>
+  <si>
+    <t>Lower stress by all possible means</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accompany their clients to help manage requirements and challenges in their environment. And be able to identify cultural difference in action.
+</t>
   </si>
   <si>
     <t>Empathy, non-judgment, hope</t>
@@ -865,6 +1059,37 @@
   </si>
   <si>
     <t>1. Cultural awareness and cultural humility when interacting with people from diverse backgrounds. This should shape the attitude of the frontline workers and help them prioritize the needs of their target population.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I have identified the main principles above. 
+In terms of personal beliefs, attitudes, values and motivations, my approach is not to identify these as if they are 'external' skills that need to be acquired by 'gimmicky' "skills training exercises" (e.g. like riding a bicycle). Instead, they should be the product of a proper, substantial and in-depth training (that includes didactic and experiential modes of learning, plus application and supervision over time), and they should not be the product of an odd weekend course that is called 'training'. 
+</t>
+  </si>
+  <si>
+    <t>equality/equity with the client</t>
+  </si>
+  <si>
+    <t>1) unconscious bias work
+2) self reflection on their journey with their own personal values, bias, motivations
+3) ability to reflect and question themselves</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) respect  for the ASM;
+2) patience,availability and willingness to help; 
+3) sensitivity to important cultural factors and beliefs;
+4) willingness to listen to the ASM stories;
+5) beliefs in the human rights of the ASM
+</t>
+  </si>
+  <si>
+    <t>1. commitment to anti-racism and anti-colonialism; 2. willingness to bend and defy Home Office rules; 3. support for the person's asylum application</t>
+  </si>
+  <si>
+    <t>Yes, and be human / show their humanity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Most important, frontline workers need to demonstrate their respect for the client, and have an attitude of checking whether it is okay to speak about certain topics in their culture. They also need to be able to have curiosity and be careful about making assumptions about the clients, belief, behaviors, feelings.
+</t>
   </si>
 </sst>
 </file>
@@ -1020,10 +1245,10 @@
         <v>45299.34706018519</v>
       </c>
       <c r="D2" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="E2" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="F2" t="n">
         <v>100.0</v>
@@ -1032,13 +1257,13 @@
         <v>270.0</v>
       </c>
       <c r="H2" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="I2" t="n" s="2">
         <v>45299.34707175926</v>
       </c>
       <c r="J2" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="K2" t="e">
         <v>#N/A</v>
@@ -1050,22 +1275,22 @@
         <v>12.5298</v>
       </c>
       <c r="N2" t="s">
-        <v>91</v>
+        <v>115</v>
       </c>
       <c r="O2" t="s">
-        <v>92</v>
+        <v>116</v>
       </c>
       <c r="P2" t="s">
-        <v>93</v>
+        <v>117</v>
       </c>
       <c r="Q2" t="s">
-        <v>94</v>
+        <v>119</v>
       </c>
       <c r="R2" t="e">
         <v>#N/A</v>
       </c>
       <c r="S2" t="s">
-        <v>100</v>
+        <v>125</v>
       </c>
       <c r="T2" t="e">
         <v>#N/A</v>
@@ -1074,31 +1299,31 @@
         <v>15.0</v>
       </c>
       <c r="V2" t="s">
-        <v>103</v>
+        <v>128</v>
       </c>
       <c r="W2" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
       <c r="X2" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
       <c r="Y2" t="s">
-        <v>108</v>
+        <v>132</v>
       </c>
       <c r="Z2" t="s">
-        <v>128</v>
+        <v>159</v>
       </c>
       <c r="AA2" t="s">
-        <v>148</v>
+        <v>186</v>
       </c>
       <c r="AB2" t="s">
-        <v>152</v>
+        <v>190</v>
       </c>
       <c r="AC2" t="s">
-        <v>172</v>
+        <v>217</v>
       </c>
       <c r="AD2" t="s">
-        <v>192</v>
+        <v>244</v>
       </c>
     </row>
     <row r="3">
@@ -1112,10 +1337,10 @@
         <v>45299.356840277775</v>
       </c>
       <c r="D3" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="E3" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="F3" t="n">
         <v>100.0</v>
@@ -1124,13 +1349,13 @@
         <v>1822.0</v>
       </c>
       <c r="H3" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="I3" t="n" s="2">
         <v>45299.35685185185</v>
       </c>
       <c r="J3" t="s">
-        <v>72</v>
+        <v>88</v>
       </c>
       <c r="K3" t="e">
         <v>#N/A</v>
@@ -1142,22 +1367,22 @@
         <v>4.9922</v>
       </c>
       <c r="N3" t="s">
-        <v>91</v>
+        <v>115</v>
       </c>
       <c r="O3" t="s">
-        <v>92</v>
+        <v>116</v>
       </c>
       <c r="P3" t="s">
-        <v>93</v>
+        <v>117</v>
       </c>
       <c r="Q3" t="s">
-        <v>94</v>
+        <v>119</v>
       </c>
       <c r="R3" t="e">
         <v>#N/A</v>
       </c>
       <c r="S3" t="s">
-        <v>101</v>
+        <v>126</v>
       </c>
       <c r="T3" t="e">
         <v>#N/A</v>
@@ -1166,31 +1391,31 @@
         <v>17.0</v>
       </c>
       <c r="V3" t="s">
-        <v>103</v>
+        <v>128</v>
       </c>
       <c r="W3" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
       <c r="X3" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
       <c r="Y3" t="s">
-        <v>109</v>
+        <v>133</v>
       </c>
       <c r="Z3" t="s">
-        <v>129</v>
+        <v>160</v>
       </c>
       <c r="AA3" t="s">
-        <v>149</v>
+        <v>187</v>
       </c>
       <c r="AB3" t="s">
-        <v>153</v>
+        <v>191</v>
       </c>
       <c r="AC3" t="s">
-        <v>173</v>
+        <v>218</v>
       </c>
       <c r="AD3" t="s">
-        <v>193</v>
+        <v>245</v>
       </c>
     </row>
     <row r="4">
@@ -1204,10 +1429,10 @@
         <v>45299.41439814815</v>
       </c>
       <c r="D4" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="E4" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="F4" t="n">
         <v>100.0</v>
@@ -1216,13 +1441,13 @@
         <v>3842.0</v>
       </c>
       <c r="H4" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="I4" t="n" s="2">
         <v>45299.41440972222</v>
       </c>
       <c r="J4" t="s">
-        <v>73</v>
+        <v>89</v>
       </c>
       <c r="K4" t="e">
         <v>#N/A</v>
@@ -1234,22 +1459,22 @@
         <v>4.7027</v>
       </c>
       <c r="N4" t="s">
-        <v>91</v>
+        <v>115</v>
       </c>
       <c r="O4" t="s">
-        <v>92</v>
+        <v>116</v>
       </c>
       <c r="P4" t="s">
-        <v>93</v>
+        <v>117</v>
       </c>
       <c r="Q4" t="s">
-        <v>95</v>
+        <v>120</v>
       </c>
       <c r="R4" t="e">
         <v>#N/A</v>
       </c>
       <c r="S4" t="s">
-        <v>102</v>
+        <v>127</v>
       </c>
       <c r="T4" t="e">
         <v>#N/A</v>
@@ -1258,31 +1483,31 @@
         <v>20.0</v>
       </c>
       <c r="V4" t="s">
-        <v>103</v>
+        <v>128</v>
       </c>
       <c r="W4" t="s">
-        <v>93</v>
+        <v>117</v>
       </c>
       <c r="X4" t="s">
-        <v>93</v>
+        <v>117</v>
       </c>
       <c r="Y4" t="s">
-        <v>110</v>
+        <v>134</v>
       </c>
       <c r="Z4" t="s">
-        <v>130</v>
+        <v>161</v>
       </c>
       <c r="AA4" t="s">
-        <v>148</v>
+        <v>186</v>
       </c>
       <c r="AB4" t="s">
-        <v>154</v>
+        <v>192</v>
       </c>
       <c r="AC4" t="s">
-        <v>174</v>
+        <v>219</v>
       </c>
       <c r="AD4" t="s">
-        <v>194</v>
+        <v>246</v>
       </c>
     </row>
     <row r="5">
@@ -1296,10 +1521,10 @@
         <v>45299.57168981481</v>
       </c>
       <c r="D5" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="E5" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="F5" t="n">
         <v>100.0</v>
@@ -1308,13 +1533,13 @@
         <v>305.0</v>
       </c>
       <c r="H5" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="I5" t="n" s="2">
         <v>45299.57170138889</v>
       </c>
       <c r="J5" t="s">
-        <v>74</v>
+        <v>90</v>
       </c>
       <c r="K5" t="e">
         <v>#N/A</v>
@@ -1326,22 +1551,22 @@
         <v>-0.0373</v>
       </c>
       <c r="N5" t="s">
-        <v>91</v>
+        <v>115</v>
       </c>
       <c r="O5" t="s">
-        <v>92</v>
+        <v>116</v>
       </c>
       <c r="P5" t="s">
-        <v>93</v>
+        <v>117</v>
       </c>
       <c r="Q5" t="s">
-        <v>95</v>
+        <v>120</v>
       </c>
       <c r="R5" t="e">
         <v>#N/A</v>
       </c>
       <c r="S5" t="s">
-        <v>100</v>
+        <v>125</v>
       </c>
       <c r="T5" t="e">
         <v>#N/A</v>
@@ -1350,31 +1575,31 @@
         <v>20.0</v>
       </c>
       <c r="V5" t="s">
-        <v>103</v>
+        <v>128</v>
       </c>
       <c r="W5" t="s">
-        <v>93</v>
+        <v>117</v>
       </c>
       <c r="X5" t="s">
-        <v>93</v>
+        <v>117</v>
       </c>
       <c r="Y5" t="s">
-        <v>111</v>
+        <v>135</v>
       </c>
       <c r="Z5" t="s">
-        <v>131</v>
+        <v>162</v>
       </c>
       <c r="AA5" t="s">
-        <v>148</v>
+        <v>186</v>
       </c>
       <c r="AB5" t="s">
-        <v>155</v>
+        <v>193</v>
       </c>
       <c r="AC5" t="s">
-        <v>175</v>
+        <v>220</v>
       </c>
       <c r="AD5" t="s">
-        <v>195</v>
+        <v>247</v>
       </c>
     </row>
     <row r="6">
@@ -1388,10 +1613,10 @@
         <v>45299.59695601852</v>
       </c>
       <c r="D6" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="E6" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="F6" t="n">
         <v>100.0</v>
@@ -1400,13 +1625,13 @@
         <v>1150.0</v>
       </c>
       <c r="H6" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="I6" t="n" s="2">
         <v>45299.59697916667</v>
       </c>
       <c r="J6" t="s">
-        <v>75</v>
+        <v>91</v>
       </c>
       <c r="K6" t="e">
         <v>#N/A</v>
@@ -1418,22 +1643,22 @@
         <v>-73.9763</v>
       </c>
       <c r="N6" t="s">
-        <v>91</v>
+        <v>115</v>
       </c>
       <c r="O6" t="s">
-        <v>92</v>
+        <v>116</v>
       </c>
       <c r="P6" t="s">
-        <v>93</v>
+        <v>117</v>
       </c>
       <c r="Q6" t="s">
-        <v>94</v>
+        <v>119</v>
       </c>
       <c r="R6" t="e">
         <v>#N/A</v>
       </c>
       <c r="S6" t="s">
-        <v>101</v>
+        <v>126</v>
       </c>
       <c r="T6" t="e">
         <v>#N/A</v>
@@ -1442,31 +1667,31 @@
         <v>20.0</v>
       </c>
       <c r="V6" t="s">
-        <v>104</v>
+        <v>129</v>
       </c>
       <c r="W6" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
       <c r="X6" t="s">
-        <v>93</v>
+        <v>117</v>
       </c>
       <c r="Y6" t="s">
-        <v>112</v>
+        <v>136</v>
       </c>
       <c r="Z6" t="s">
-        <v>132</v>
+        <v>163</v>
       </c>
       <c r="AA6" t="s">
-        <v>148</v>
+        <v>186</v>
       </c>
       <c r="AB6" t="s">
-        <v>156</v>
+        <v>194</v>
       </c>
       <c r="AC6" t="s">
-        <v>176</v>
+        <v>221</v>
       </c>
       <c r="AD6" t="s">
-        <v>196</v>
+        <v>248</v>
       </c>
     </row>
     <row r="7">
@@ -1480,10 +1705,10 @@
         <v>45299.68324074074</v>
       </c>
       <c r="D7" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="E7" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="F7" t="n">
         <v>100.0</v>
@@ -1492,13 +1717,13 @@
         <v>489.0</v>
       </c>
       <c r="H7" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="I7" t="n" s="2">
         <v>45299.68325231482</v>
       </c>
       <c r="J7" t="s">
-        <v>76</v>
+        <v>92</v>
       </c>
       <c r="K7" t="e">
         <v>#N/A</v>
@@ -1510,22 +1735,22 @@
         <v>-123.1234</v>
       </c>
       <c r="N7" t="s">
-        <v>91</v>
+        <v>115</v>
       </c>
       <c r="O7" t="s">
-        <v>92</v>
+        <v>116</v>
       </c>
       <c r="P7" t="s">
-        <v>93</v>
+        <v>117</v>
       </c>
       <c r="Q7" t="s">
-        <v>94</v>
+        <v>119</v>
       </c>
       <c r="R7" t="e">
         <v>#N/A</v>
       </c>
       <c r="S7" t="s">
-        <v>102</v>
+        <v>127</v>
       </c>
       <c r="T7" t="e">
         <v>#N/A</v>
@@ -1534,31 +1759,31 @@
         <v>25.0</v>
       </c>
       <c r="V7" t="s">
-        <v>104</v>
+        <v>129</v>
       </c>
       <c r="W7" t="s">
-        <v>93</v>
+        <v>117</v>
       </c>
       <c r="X7" t="s">
-        <v>93</v>
+        <v>117</v>
       </c>
       <c r="Y7" t="s">
-        <v>113</v>
+        <v>137</v>
       </c>
       <c r="Z7" t="s">
-        <v>133</v>
+        <v>164</v>
       </c>
       <c r="AA7" t="s">
-        <v>150</v>
+        <v>188</v>
       </c>
       <c r="AB7" t="s">
-        <v>157</v>
+        <v>195</v>
       </c>
       <c r="AC7" t="s">
-        <v>177</v>
+        <v>222</v>
       </c>
       <c r="AD7" t="s">
-        <v>197</v>
+        <v>249</v>
       </c>
     </row>
     <row r="8">
@@ -1572,10 +1797,10 @@
         <v>45300.07512731482</v>
       </c>
       <c r="D8" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="E8" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="F8" t="n">
         <v>100.0</v>
@@ -1584,13 +1809,13 @@
         <v>45086.0</v>
       </c>
       <c r="H8" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="I8" t="n" s="2">
         <v>45300.07513888889</v>
       </c>
       <c r="J8" t="s">
-        <v>77</v>
+        <v>93</v>
       </c>
       <c r="K8" t="e">
         <v>#N/A</v>
@@ -1602,22 +1827,22 @@
         <v>150.7782</v>
       </c>
       <c r="N8" t="s">
-        <v>91</v>
+        <v>115</v>
       </c>
       <c r="O8" t="s">
-        <v>92</v>
+        <v>116</v>
       </c>
       <c r="P8" t="s">
-        <v>93</v>
+        <v>117</v>
       </c>
       <c r="Q8" t="s">
-        <v>94</v>
+        <v>119</v>
       </c>
       <c r="R8" t="e">
         <v>#N/A</v>
       </c>
       <c r="S8" t="s">
-        <v>100</v>
+        <v>125</v>
       </c>
       <c r="T8" t="e">
         <v>#N/A</v>
@@ -1626,31 +1851,31 @@
         <v>20.0</v>
       </c>
       <c r="V8" t="s">
-        <v>105</v>
+        <v>130</v>
       </c>
       <c r="W8" t="s">
-        <v>93</v>
+        <v>117</v>
       </c>
       <c r="X8" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
       <c r="Y8" t="s">
-        <v>114</v>
+        <v>138</v>
       </c>
       <c r="Z8" t="s">
-        <v>134</v>
+        <v>165</v>
       </c>
       <c r="AA8" t="s">
-        <v>151</v>
+        <v>189</v>
       </c>
       <c r="AB8" t="s">
-        <v>158</v>
+        <v>196</v>
       </c>
       <c r="AC8" t="s">
-        <v>178</v>
+        <v>223</v>
       </c>
       <c r="AD8" t="s">
-        <v>198</v>
+        <v>250</v>
       </c>
     </row>
     <row r="9">
@@ -1664,10 +1889,10 @@
         <v>45300.39530092593</v>
       </c>
       <c r="D9" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="E9" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="F9" t="n">
         <v>100.0</v>
@@ -1676,13 +1901,13 @@
         <v>805.0</v>
       </c>
       <c r="H9" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="I9" t="n" s="2">
         <v>45300.3953125</v>
       </c>
       <c r="J9" t="s">
-        <v>78</v>
+        <v>94</v>
       </c>
       <c r="K9" t="e">
         <v>#N/A</v>
@@ -1694,22 +1919,22 @@
         <v>5.1907</v>
       </c>
       <c r="N9" t="s">
-        <v>91</v>
+        <v>115</v>
       </c>
       <c r="O9" t="s">
-        <v>92</v>
+        <v>116</v>
       </c>
       <c r="P9" t="s">
-        <v>93</v>
+        <v>117</v>
       </c>
       <c r="Q9" t="s">
-        <v>95</v>
+        <v>120</v>
       </c>
       <c r="R9" t="e">
         <v>#N/A</v>
       </c>
       <c r="S9" t="s">
-        <v>100</v>
+        <v>125</v>
       </c>
       <c r="T9" t="e">
         <v>#N/A</v>
@@ -1718,31 +1943,31 @@
         <v>25.0</v>
       </c>
       <c r="V9" t="s">
-        <v>103</v>
+        <v>128</v>
       </c>
       <c r="W9" t="s">
-        <v>93</v>
+        <v>117</v>
       </c>
       <c r="X9" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
       <c r="Y9" t="s">
-        <v>115</v>
+        <v>139</v>
       </c>
       <c r="Z9" t="s">
-        <v>135</v>
+        <v>166</v>
       </c>
       <c r="AA9" t="s">
-        <v>151</v>
+        <v>189</v>
       </c>
       <c r="AB9" t="s">
-        <v>159</v>
+        <v>197</v>
       </c>
       <c r="AC9" t="s">
-        <v>179</v>
+        <v>224</v>
       </c>
       <c r="AD9" t="s">
-        <v>199</v>
+        <v>251</v>
       </c>
     </row>
     <row r="10">
@@ -1756,10 +1981,10 @@
         <v>45300.417349537034</v>
       </c>
       <c r="D10" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="E10" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="F10" t="n">
         <v>100.0</v>
@@ -1768,13 +1993,13 @@
         <v>1391.0</v>
       </c>
       <c r="H10" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="I10" t="n" s="2">
         <v>45300.41736111111</v>
       </c>
       <c r="J10" t="s">
-        <v>79</v>
+        <v>95</v>
       </c>
       <c r="K10" t="e">
         <v>#N/A</v>
@@ -1786,22 +2011,22 @@
         <v>4.8777</v>
       </c>
       <c r="N10" t="s">
-        <v>91</v>
+        <v>115</v>
       </c>
       <c r="O10" t="s">
-        <v>92</v>
+        <v>116</v>
       </c>
       <c r="P10" t="s">
-        <v>93</v>
+        <v>117</v>
       </c>
       <c r="Q10" t="s">
-        <v>94</v>
+        <v>119</v>
       </c>
       <c r="R10" t="e">
         <v>#N/A</v>
       </c>
       <c r="S10" t="s">
-        <v>102</v>
+        <v>127</v>
       </c>
       <c r="T10" t="e">
         <v>#N/A</v>
@@ -1810,31 +2035,31 @@
         <v>5.0</v>
       </c>
       <c r="V10" t="s">
-        <v>103</v>
+        <v>128</v>
       </c>
       <c r="W10" t="s">
-        <v>93</v>
+        <v>117</v>
       </c>
       <c r="X10" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
       <c r="Y10" t="s">
-        <v>116</v>
+        <v>140</v>
       </c>
       <c r="Z10" t="s">
-        <v>136</v>
+        <v>167</v>
       </c>
       <c r="AA10" t="s">
-        <v>148</v>
+        <v>186</v>
       </c>
       <c r="AB10" t="s">
-        <v>160</v>
+        <v>198</v>
       </c>
       <c r="AC10" t="s">
-        <v>180</v>
+        <v>225</v>
       </c>
       <c r="AD10" t="s">
-        <v>200</v>
+        <v>252</v>
       </c>
     </row>
     <row r="11">
@@ -1848,10 +2073,10 @@
         <v>45300.53320601852</v>
       </c>
       <c r="D11" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="E11" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="F11" t="n">
         <v>100.0</v>
@@ -1860,13 +2085,13 @@
         <v>103625.0</v>
       </c>
       <c r="H11" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="I11" t="n" s="2">
         <v>45300.533217592594</v>
       </c>
       <c r="J11" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="K11" t="e">
         <v>#N/A</v>
@@ -1878,22 +2103,22 @@
         <v>4.3356</v>
       </c>
       <c r="N11" t="s">
-        <v>91</v>
+        <v>115</v>
       </c>
       <c r="O11" t="s">
-        <v>92</v>
+        <v>116</v>
       </c>
       <c r="P11" t="s">
-        <v>93</v>
+        <v>117</v>
       </c>
       <c r="Q11" t="s">
-        <v>95</v>
+        <v>120</v>
       </c>
       <c r="R11" t="e">
         <v>#N/A</v>
       </c>
       <c r="S11" t="s">
-        <v>102</v>
+        <v>127</v>
       </c>
       <c r="T11" t="e">
         <v>#N/A</v>
@@ -1902,31 +2127,31 @@
         <v>4.0</v>
       </c>
       <c r="V11" t="s">
-        <v>103</v>
+        <v>128</v>
       </c>
       <c r="W11" t="s">
-        <v>93</v>
+        <v>117</v>
       </c>
       <c r="X11" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
       <c r="Y11" t="s">
-        <v>117</v>
+        <v>141</v>
       </c>
       <c r="Z11" t="s">
-        <v>137</v>
+        <v>168</v>
       </c>
       <c r="AA11" t="s">
-        <v>148</v>
+        <v>186</v>
       </c>
       <c r="AB11" t="s">
-        <v>161</v>
+        <v>199</v>
       </c>
       <c r="AC11" t="s">
-        <v>181</v>
+        <v>226</v>
       </c>
       <c r="AD11" t="s">
-        <v>201</v>
+        <v>253</v>
       </c>
     </row>
     <row r="12">
@@ -1940,10 +2165,10 @@
         <v>45300.66453703704</v>
       </c>
       <c r="D12" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="E12" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="F12" t="n">
         <v>100.0</v>
@@ -1952,13 +2177,13 @@
         <v>2065.0</v>
       </c>
       <c r="H12" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="I12" t="n" s="2">
         <v>45300.66454861111</v>
       </c>
       <c r="J12" t="s">
-        <v>81</v>
+        <v>97</v>
       </c>
       <c r="K12" t="e">
         <v>#N/A</v>
@@ -1970,22 +2195,22 @@
         <v>-80.843</v>
       </c>
       <c r="N12" t="s">
-        <v>91</v>
+        <v>115</v>
       </c>
       <c r="O12" t="s">
-        <v>92</v>
+        <v>116</v>
       </c>
       <c r="P12" t="s">
-        <v>93</v>
+        <v>117</v>
       </c>
       <c r="Q12" t="s">
-        <v>96</v>
+        <v>121</v>
       </c>
       <c r="R12" t="e">
         <v>#N/A</v>
       </c>
       <c r="S12" t="s">
-        <v>102</v>
+        <v>127</v>
       </c>
       <c r="T12" t="e">
         <v>#N/A</v>
@@ -1994,31 +2219,31 @@
         <v>30.0</v>
       </c>
       <c r="V12" t="s">
-        <v>104</v>
+        <v>129</v>
       </c>
       <c r="W12" t="s">
-        <v>93</v>
+        <v>117</v>
       </c>
       <c r="X12" t="s">
-        <v>93</v>
+        <v>117</v>
       </c>
       <c r="Y12" t="s">
-        <v>118</v>
+        <v>142</v>
       </c>
       <c r="Z12" t="s">
-        <v>138</v>
+        <v>169</v>
       </c>
       <c r="AA12" t="s">
-        <v>148</v>
+        <v>186</v>
       </c>
       <c r="AB12" t="s">
-        <v>162</v>
+        <v>200</v>
       </c>
       <c r="AC12" t="s">
-        <v>182</v>
+        <v>227</v>
       </c>
       <c r="AD12" t="s">
-        <v>202</v>
+        <v>254</v>
       </c>
     </row>
     <row r="13">
@@ -2032,10 +2257,10 @@
         <v>45300.88851851852</v>
       </c>
       <c r="D13" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="E13" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="F13" t="n">
         <v>100.0</v>
@@ -2044,13 +2269,13 @@
         <v>1147.0</v>
       </c>
       <c r="H13" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="I13" t="n" s="2">
         <v>45300.88854166667</v>
       </c>
       <c r="J13" t="s">
-        <v>82</v>
+        <v>98</v>
       </c>
       <c r="K13" t="e">
         <v>#N/A</v>
@@ -2062,22 +2287,22 @@
         <v>5.2577</v>
       </c>
       <c r="N13" t="s">
-        <v>91</v>
+        <v>115</v>
       </c>
       <c r="O13" t="s">
-        <v>92</v>
+        <v>116</v>
       </c>
       <c r="P13" t="s">
-        <v>93</v>
+        <v>117</v>
       </c>
       <c r="Q13" t="s">
-        <v>97</v>
+        <v>122</v>
       </c>
       <c r="R13" t="e">
         <v>#N/A</v>
       </c>
       <c r="S13" t="s">
-        <v>101</v>
+        <v>126</v>
       </c>
       <c r="T13" t="e">
         <v>#N/A</v>
@@ -2086,31 +2311,31 @@
         <v>20.0</v>
       </c>
       <c r="V13" t="s">
-        <v>103</v>
+        <v>128</v>
       </c>
       <c r="W13" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
       <c r="X13" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
       <c r="Y13" t="s">
-        <v>119</v>
+        <v>143</v>
       </c>
       <c r="Z13" t="s">
-        <v>139</v>
+        <v>170</v>
       </c>
       <c r="AA13" t="s">
-        <v>148</v>
+        <v>186</v>
       </c>
       <c r="AB13" t="s">
-        <v>163</v>
+        <v>201</v>
       </c>
       <c r="AC13" t="s">
-        <v>183</v>
+        <v>228</v>
       </c>
       <c r="AD13" t="s">
-        <v>203</v>
+        <v>255</v>
       </c>
     </row>
     <row r="14">
@@ -2124,10 +2349,10 @@
         <v>45301.86099537037</v>
       </c>
       <c r="D14" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="E14" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="F14" t="n">
         <v>100.0</v>
@@ -2136,13 +2361,13 @@
         <v>69113.0</v>
       </c>
       <c r="H14" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="I14" t="n" s="2">
         <v>45301.86100694444</v>
       </c>
       <c r="J14" t="s">
-        <v>83</v>
+        <v>99</v>
       </c>
       <c r="K14" t="e">
         <v>#N/A</v>
@@ -2154,22 +2379,22 @@
         <v>-77.5546</v>
       </c>
       <c r="N14" t="s">
-        <v>91</v>
+        <v>115</v>
       </c>
       <c r="O14" t="s">
-        <v>92</v>
+        <v>116</v>
       </c>
       <c r="P14" t="s">
-        <v>93</v>
+        <v>117</v>
       </c>
       <c r="Q14" t="s">
-        <v>94</v>
+        <v>119</v>
       </c>
       <c r="R14" t="e">
         <v>#N/A</v>
       </c>
       <c r="S14" t="s">
-        <v>102</v>
+        <v>127</v>
       </c>
       <c r="T14" t="e">
         <v>#N/A</v>
@@ -2178,31 +2403,31 @@
         <v>21.0</v>
       </c>
       <c r="V14" t="s">
-        <v>104</v>
+        <v>129</v>
       </c>
       <c r="W14" t="s">
-        <v>93</v>
+        <v>117</v>
       </c>
       <c r="X14" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
       <c r="Y14" t="s">
-        <v>120</v>
+        <v>144</v>
       </c>
       <c r="Z14" t="s">
-        <v>140</v>
+        <v>171</v>
       </c>
       <c r="AA14" t="s">
-        <v>151</v>
+        <v>189</v>
       </c>
       <c r="AB14" t="s">
-        <v>164</v>
+        <v>202</v>
       </c>
       <c r="AC14" t="s">
-        <v>184</v>
+        <v>229</v>
       </c>
       <c r="AD14" t="s">
-        <v>204</v>
+        <v>256</v>
       </c>
     </row>
     <row r="15">
@@ -2216,10 +2441,10 @@
         <v>45303.72300925926</v>
       </c>
       <c r="D15" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="E15" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="F15" t="n">
         <v>100.0</v>
@@ -2228,13 +2453,13 @@
         <v>957.0</v>
       </c>
       <c r="H15" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="I15" t="n" s="2">
         <v>45303.723020833335</v>
       </c>
       <c r="J15" t="s">
-        <v>84</v>
+        <v>100</v>
       </c>
       <c r="K15" t="e">
         <v>#N/A</v>
@@ -2246,22 +2471,22 @@
         <v>18.0517</v>
       </c>
       <c r="N15" t="s">
-        <v>91</v>
+        <v>115</v>
       </c>
       <c r="O15" t="s">
-        <v>92</v>
+        <v>116</v>
       </c>
       <c r="P15" t="s">
-        <v>93</v>
+        <v>117</v>
       </c>
       <c r="Q15" t="s">
-        <v>94</v>
+        <v>119</v>
       </c>
       <c r="R15" t="e">
         <v>#N/A</v>
       </c>
       <c r="S15" t="s">
-        <v>102</v>
+        <v>127</v>
       </c>
       <c r="T15" t="e">
         <v>#N/A</v>
@@ -2270,31 +2495,31 @@
         <v>30.0</v>
       </c>
       <c r="V15" t="s">
-        <v>103</v>
+        <v>128</v>
       </c>
       <c r="W15" t="s">
-        <v>93</v>
+        <v>117</v>
       </c>
       <c r="X15" t="s">
-        <v>93</v>
+        <v>117</v>
       </c>
       <c r="Y15" t="s">
-        <v>121</v>
+        <v>145</v>
       </c>
       <c r="Z15" t="s">
-        <v>141</v>
+        <v>172</v>
       </c>
       <c r="AA15" t="s">
-        <v>150</v>
+        <v>188</v>
       </c>
       <c r="AB15" t="s">
-        <v>165</v>
+        <v>203</v>
       </c>
       <c r="AC15" t="s">
-        <v>185</v>
+        <v>230</v>
       </c>
       <c r="AD15" t="s">
-        <v>205</v>
+        <v>257</v>
       </c>
     </row>
     <row r="16">
@@ -2308,10 +2533,10 @@
         <v>45304.01983796296</v>
       </c>
       <c r="D16" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="E16" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="F16" t="n">
         <v>100.0</v>
@@ -2320,13 +2545,13 @@
         <v>3389.0</v>
       </c>
       <c r="H16" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="I16" t="n" s="2">
         <v>45304.01984953704</v>
       </c>
       <c r="J16" t="s">
-        <v>85</v>
+        <v>101</v>
       </c>
       <c r="K16" t="e">
         <v>#N/A</v>
@@ -2338,22 +2563,22 @@
         <v>-79.188</v>
       </c>
       <c r="N16" t="s">
-        <v>91</v>
+        <v>115</v>
       </c>
       <c r="O16" t="s">
-        <v>92</v>
+        <v>116</v>
       </c>
       <c r="P16" t="s">
-        <v>93</v>
+        <v>117</v>
       </c>
       <c r="Q16" t="s">
-        <v>95</v>
+        <v>120</v>
       </c>
       <c r="R16" t="e">
         <v>#N/A</v>
       </c>
       <c r="S16" t="s">
-        <v>102</v>
+        <v>127</v>
       </c>
       <c r="T16" t="e">
         <v>#N/A</v>
@@ -2362,31 +2587,31 @@
         <v>30.0</v>
       </c>
       <c r="V16" t="s">
-        <v>104</v>
+        <v>129</v>
       </c>
       <c r="W16" t="s">
-        <v>93</v>
+        <v>117</v>
       </c>
       <c r="X16" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
       <c r="Y16" t="s">
-        <v>122</v>
+        <v>146</v>
       </c>
       <c r="Z16" t="s">
-        <v>142</v>
+        <v>173</v>
       </c>
       <c r="AA16" t="s">
-        <v>148</v>
+        <v>186</v>
       </c>
       <c r="AB16" t="s">
-        <v>166</v>
+        <v>204</v>
       </c>
       <c r="AC16" t="s">
-        <v>186</v>
+        <v>231</v>
       </c>
       <c r="AD16" t="s">
-        <v>206</v>
+        <v>258</v>
       </c>
     </row>
     <row r="17">
@@ -2400,10 +2625,10 @@
         <v>45306.346180555556</v>
       </c>
       <c r="D17" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="E17" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="F17" t="n">
         <v>100.0</v>
@@ -2412,13 +2637,13 @@
         <v>4101.0</v>
       </c>
       <c r="H17" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="I17" t="n" s="2">
         <v>45306.346192129626</v>
       </c>
       <c r="J17" t="s">
-        <v>86</v>
+        <v>102</v>
       </c>
       <c r="K17" t="e">
         <v>#N/A</v>
@@ -2430,22 +2655,22 @@
         <v>51.5321</v>
       </c>
       <c r="N17" t="s">
-        <v>91</v>
+        <v>115</v>
       </c>
       <c r="O17" t="s">
-        <v>92</v>
+        <v>116</v>
       </c>
       <c r="P17" t="s">
-        <v>93</v>
+        <v>117</v>
       </c>
       <c r="Q17" t="s">
-        <v>96</v>
+        <v>121</v>
       </c>
       <c r="R17" t="e">
         <v>#N/A</v>
       </c>
       <c r="S17" t="s">
-        <v>100</v>
+        <v>125</v>
       </c>
       <c r="T17" t="e">
         <v>#N/A</v>
@@ -2454,31 +2679,31 @@
         <v>26.0</v>
       </c>
       <c r="V17" t="s">
-        <v>105</v>
+        <v>130</v>
       </c>
       <c r="W17" t="s">
-        <v>93</v>
+        <v>117</v>
       </c>
       <c r="X17" t="s">
-        <v>93</v>
+        <v>117</v>
       </c>
       <c r="Y17" t="s">
-        <v>123</v>
+        <v>147</v>
       </c>
       <c r="Z17" t="s">
-        <v>143</v>
+        <v>174</v>
       </c>
       <c r="AA17" t="s">
-        <v>151</v>
+        <v>189</v>
       </c>
       <c r="AB17" t="s">
-        <v>167</v>
+        <v>205</v>
       </c>
       <c r="AC17" t="s">
-        <v>187</v>
+        <v>232</v>
       </c>
       <c r="AD17" t="s">
-        <v>207</v>
+        <v>259</v>
       </c>
     </row>
     <row r="18">
@@ -2492,10 +2717,10 @@
         <v>45306.36274305556</v>
       </c>
       <c r="D18" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="E18" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="F18" t="n">
         <v>100.0</v>
@@ -2504,13 +2729,13 @@
         <v>600161.0</v>
       </c>
       <c r="H18" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="I18" t="n" s="2">
         <v>45306.362754629634</v>
       </c>
       <c r="J18" t="s">
-        <v>87</v>
+        <v>103</v>
       </c>
       <c r="K18" t="e">
         <v>#N/A</v>
@@ -2522,22 +2747,22 @@
         <v>8.5671</v>
       </c>
       <c r="N18" t="s">
-        <v>91</v>
+        <v>115</v>
       </c>
       <c r="O18" t="s">
-        <v>92</v>
+        <v>116</v>
       </c>
       <c r="P18" t="s">
-        <v>93</v>
+        <v>117</v>
       </c>
       <c r="Q18" t="s">
-        <v>98</v>
+        <v>123</v>
       </c>
       <c r="R18" t="s">
-        <v>99</v>
+        <v>124</v>
       </c>
       <c r="S18" t="s">
-        <v>102</v>
+        <v>127</v>
       </c>
       <c r="T18" t="e">
         <v>#N/A</v>
@@ -2546,31 +2771,31 @@
         <v>22.0</v>
       </c>
       <c r="V18" t="s">
-        <v>103</v>
+        <v>128</v>
       </c>
       <c r="W18" t="s">
-        <v>93</v>
+        <v>117</v>
       </c>
       <c r="X18" t="s">
-        <v>93</v>
+        <v>117</v>
       </c>
       <c r="Y18" t="s">
-        <v>124</v>
+        <v>148</v>
       </c>
       <c r="Z18" t="s">
-        <v>144</v>
+        <v>175</v>
       </c>
       <c r="AA18" t="s">
-        <v>150</v>
+        <v>188</v>
       </c>
       <c r="AB18" t="s">
-        <v>168</v>
+        <v>206</v>
       </c>
       <c r="AC18" t="s">
-        <v>188</v>
+        <v>233</v>
       </c>
       <c r="AD18" t="s">
-        <v>208</v>
+        <v>260</v>
       </c>
     </row>
     <row r="19">
@@ -2584,10 +2809,10 @@
         <v>45306.40620370371</v>
       </c>
       <c r="D19" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="E19" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="F19" t="n">
         <v>100.0</v>
@@ -2596,13 +2821,13 @@
         <v>960.0</v>
       </c>
       <c r="H19" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="I19" t="n" s="2">
         <v>45306.40621527778</v>
       </c>
       <c r="J19" t="s">
-        <v>88</v>
+        <v>104</v>
       </c>
       <c r="K19" t="e">
         <v>#N/A</v>
@@ -2614,22 +2839,22 @@
         <v>-0.066</v>
       </c>
       <c r="N19" t="s">
-        <v>91</v>
+        <v>115</v>
       </c>
       <c r="O19" t="s">
-        <v>92</v>
+        <v>116</v>
       </c>
       <c r="P19" t="s">
-        <v>93</v>
+        <v>117</v>
       </c>
       <c r="Q19" t="s">
-        <v>95</v>
+        <v>120</v>
       </c>
       <c r="R19" t="e">
         <v>#N/A</v>
       </c>
       <c r="S19" t="s">
-        <v>100</v>
+        <v>125</v>
       </c>
       <c r="T19" t="e">
         <v>#N/A</v>
@@ -2638,31 +2863,31 @@
         <v>15.0</v>
       </c>
       <c r="V19" t="s">
-        <v>106</v>
+        <v>131</v>
       </c>
       <c r="W19" t="s">
-        <v>93</v>
+        <v>117</v>
       </c>
       <c r="X19" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
       <c r="Y19" t="s">
-        <v>125</v>
+        <v>149</v>
       </c>
       <c r="Z19" t="s">
-        <v>145</v>
+        <v>176</v>
       </c>
       <c r="AA19" t="s">
-        <v>148</v>
+        <v>186</v>
       </c>
       <c r="AB19" t="s">
-        <v>169</v>
+        <v>207</v>
       </c>
       <c r="AC19" t="s">
-        <v>189</v>
+        <v>234</v>
       </c>
       <c r="AD19" t="s">
-        <v>209</v>
+        <v>261</v>
       </c>
     </row>
     <row r="20">
@@ -2676,10 +2901,10 @@
         <v>45306.474270833336</v>
       </c>
       <c r="D20" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="E20" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="F20" t="n">
         <v>100.0</v>
@@ -2688,13 +2913,13 @@
         <v>8378.0</v>
       </c>
       <c r="H20" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="I20" t="n" s="2">
         <v>45306.474282407406</v>
       </c>
       <c r="J20" t="s">
-        <v>89</v>
+        <v>105</v>
       </c>
       <c r="K20" t="e">
         <v>#N/A</v>
@@ -2706,22 +2931,22 @@
         <v>-0.1235</v>
       </c>
       <c r="N20" t="s">
-        <v>91</v>
+        <v>115</v>
       </c>
       <c r="O20" t="s">
-        <v>92</v>
+        <v>116</v>
       </c>
       <c r="P20" t="s">
-        <v>93</v>
+        <v>117</v>
       </c>
       <c r="Q20" t="s">
-        <v>95</v>
+        <v>120</v>
       </c>
       <c r="R20" t="e">
         <v>#N/A</v>
       </c>
       <c r="S20" t="s">
-        <v>100</v>
+        <v>125</v>
       </c>
       <c r="T20" t="e">
         <v>#N/A</v>
@@ -2730,31 +2955,31 @@
         <v>20.0</v>
       </c>
       <c r="V20" t="s">
-        <v>103</v>
+        <v>128</v>
       </c>
       <c r="W20" t="s">
-        <v>93</v>
+        <v>117</v>
       </c>
       <c r="X20" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
       <c r="Y20" t="s">
-        <v>126</v>
+        <v>150</v>
       </c>
       <c r="Z20" t="s">
-        <v>146</v>
+        <v>177</v>
       </c>
       <c r="AA20" t="s">
-        <v>150</v>
+        <v>188</v>
       </c>
       <c r="AB20" t="s">
-        <v>170</v>
+        <v>208</v>
       </c>
       <c r="AC20" t="s">
-        <v>190</v>
+        <v>235</v>
       </c>
       <c r="AD20" t="s">
-        <v>210</v>
+        <v>262</v>
       </c>
     </row>
     <row r="21">
@@ -2768,10 +2993,10 @@
         <v>45306.49673611111</v>
       </c>
       <c r="D21" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="E21" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="F21" t="n">
         <v>100.0</v>
@@ -2780,13 +3005,13 @@
         <v>633.0</v>
       </c>
       <c r="H21" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="I21" t="n" s="2">
         <v>45306.49674768519</v>
       </c>
       <c r="J21" t="s">
-        <v>90</v>
+        <v>106</v>
       </c>
       <c r="K21" t="e">
         <v>#N/A</v>
@@ -2798,22 +3023,22 @@
         <v>5.3275</v>
       </c>
       <c r="N21" t="s">
-        <v>91</v>
+        <v>115</v>
       </c>
       <c r="O21" t="s">
-        <v>92</v>
+        <v>116</v>
       </c>
       <c r="P21" t="s">
-        <v>93</v>
+        <v>117</v>
       </c>
       <c r="Q21" t="s">
-        <v>94</v>
+        <v>119</v>
       </c>
       <c r="R21" t="e">
         <v>#N/A</v>
       </c>
       <c r="S21" t="s">
-        <v>102</v>
+        <v>127</v>
       </c>
       <c r="T21" t="e">
         <v>#N/A</v>
@@ -2822,31 +3047,755 @@
         <v>7.0</v>
       </c>
       <c r="V21" t="s">
-        <v>103</v>
+        <v>128</v>
       </c>
       <c r="W21" t="s">
-        <v>93</v>
+        <v>117</v>
       </c>
       <c r="X21" t="s">
+        <v>118</v>
+      </c>
+      <c r="Y21" t="s">
+        <v>151</v>
+      </c>
+      <c r="Z21" t="s">
+        <v>178</v>
+      </c>
+      <c r="AA21" t="s">
+        <v>186</v>
+      </c>
+      <c r="AB21" t="s">
+        <v>209</v>
+      </c>
+      <c r="AC21" t="s">
+        <v>236</v>
+      </c>
+      <c r="AD21" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>49</v>
+      </c>
+      <c r="B22" t="n" s="2">
+        <v>45306.506261574075</v>
+      </c>
+      <c r="C22" t="n" s="2">
+        <v>45306.67015046296</v>
+      </c>
+      <c r="D22" t="s">
+        <v>57</v>
+      </c>
+      <c r="E22" t="s">
+        <v>78</v>
+      </c>
+      <c r="F22" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="G22" t="n">
+        <v>14159.0</v>
+      </c>
+      <c r="H22" t="s">
+        <v>86</v>
+      </c>
+      <c r="I22" t="n" s="2">
+        <v>45306.67016203704</v>
+      </c>
+      <c r="J22" t="s">
         <v>107</v>
       </c>
-      <c r="Y21" t="s">
+      <c r="K22" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L22" t="n">
+        <v>51.5598</v>
+      </c>
+      <c r="M22" t="n">
+        <v>-0.0096</v>
+      </c>
+      <c r="N22" t="s">
+        <v>115</v>
+      </c>
+      <c r="O22" t="s">
+        <v>116</v>
+      </c>
+      <c r="P22" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>119</v>
+      </c>
+      <c r="R22" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="S22" t="s">
+        <v>125</v>
+      </c>
+      <c r="T22" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="U22" t="n">
+        <v>40.0</v>
+      </c>
+      <c r="V22" t="s">
+        <v>128</v>
+      </c>
+      <c r="W22" t="s">
+        <v>118</v>
+      </c>
+      <c r="X22" t="s">
+        <v>118</v>
+      </c>
+      <c r="Y22" t="s">
+        <v>152</v>
+      </c>
+      <c r="Z22" t="s">
+        <v>179</v>
+      </c>
+      <c r="AA22" t="s">
+        <v>188</v>
+      </c>
+      <c r="AB22" t="s">
+        <v>210</v>
+      </c>
+      <c r="AC22" t="s">
+        <v>237</v>
+      </c>
+      <c r="AD22" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B23" t="n" s="2">
+        <v>45306.82344907407</v>
+      </c>
+      <c r="C23" t="n" s="2">
+        <v>45306.826828703706</v>
+      </c>
+      <c r="D23" t="s">
+        <v>57</v>
+      </c>
+      <c r="E23" t="s">
+        <v>79</v>
+      </c>
+      <c r="F23" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="G23" t="n">
+        <v>291.0</v>
+      </c>
+      <c r="H23" t="s">
+        <v>86</v>
+      </c>
+      <c r="I23" t="n" s="2">
+        <v>45306.826840277776</v>
+      </c>
+      <c r="J23" t="s">
+        <v>108</v>
+      </c>
+      <c r="K23" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L23" t="n">
+        <v>32.6333</v>
+      </c>
+      <c r="M23" t="n">
+        <v>-16.9</v>
+      </c>
+      <c r="N23" t="s">
+        <v>115</v>
+      </c>
+      <c r="O23" t="s">
+        <v>116</v>
+      </c>
+      <c r="P23" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>119</v>
+      </c>
+      <c r="R23" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="S23" t="s">
         <v>127</v>
       </c>
-      <c r="Z21" t="s">
-        <v>147</v>
-      </c>
-      <c r="AA21" t="s">
-        <v>148</v>
-      </c>
-      <c r="AB21" t="s">
-        <v>171</v>
-      </c>
-      <c r="AC21" t="s">
-        <v>191</v>
-      </c>
-      <c r="AD21" t="s">
+      <c r="T23" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="U23" t="n">
+        <v>22.0</v>
+      </c>
+      <c r="V23" t="s">
+        <v>128</v>
+      </c>
+      <c r="W23" t="s">
+        <v>118</v>
+      </c>
+      <c r="X23" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y23" t="s">
+        <v>153</v>
+      </c>
+      <c r="Z23" t="s">
+        <v>180</v>
+      </c>
+      <c r="AA23" t="s">
+        <v>188</v>
+      </c>
+      <c r="AB23" t="s">
         <v>211</v>
+      </c>
+      <c r="AC23" t="s">
+        <v>238</v>
+      </c>
+      <c r="AD23" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>51</v>
+      </c>
+      <c r="B24" t="n" s="2">
+        <v>45307.270902777775</v>
+      </c>
+      <c r="C24" t="n" s="2">
+        <v>45307.27956018518</v>
+      </c>
+      <c r="D24" t="s">
+        <v>57</v>
+      </c>
+      <c r="E24" t="s">
+        <v>80</v>
+      </c>
+      <c r="F24" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="G24" t="n">
+        <v>747.0</v>
+      </c>
+      <c r="H24" t="s">
+        <v>86</v>
+      </c>
+      <c r="I24" t="n" s="2">
+        <v>45307.27957175926</v>
+      </c>
+      <c r="J24" t="s">
+        <v>109</v>
+      </c>
+      <c r="K24" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L24" t="n">
+        <v>51.5888</v>
+      </c>
+      <c r="M24" t="n">
+        <v>-0.0247</v>
+      </c>
+      <c r="N24" t="s">
+        <v>115</v>
+      </c>
+      <c r="O24" t="s">
+        <v>116</v>
+      </c>
+      <c r="P24" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>121</v>
+      </c>
+      <c r="R24" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="S24" t="s">
+        <v>127</v>
+      </c>
+      <c r="T24" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="U24" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="V24" t="s">
+        <v>128</v>
+      </c>
+      <c r="W24" t="s">
+        <v>117</v>
+      </c>
+      <c r="X24" t="s">
+        <v>118</v>
+      </c>
+      <c r="Y24" t="s">
+        <v>154</v>
+      </c>
+      <c r="Z24" t="s">
+        <v>181</v>
+      </c>
+      <c r="AA24" t="s">
+        <v>186</v>
+      </c>
+      <c r="AB24" t="s">
+        <v>212</v>
+      </c>
+      <c r="AC24" t="s">
+        <v>239</v>
+      </c>
+      <c r="AD24" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>52</v>
+      </c>
+      <c r="B25" t="n" s="2">
+        <v>45307.33777777778</v>
+      </c>
+      <c r="C25" t="n" s="2">
+        <v>45307.4065625</v>
+      </c>
+      <c r="D25" t="s">
+        <v>57</v>
+      </c>
+      <c r="E25" t="s">
+        <v>81</v>
+      </c>
+      <c r="F25" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="G25" t="n">
+        <v>5942.0</v>
+      </c>
+      <c r="H25" t="s">
+        <v>86</v>
+      </c>
+      <c r="I25" t="n" s="2">
+        <v>45307.40657407408</v>
+      </c>
+      <c r="J25" t="s">
+        <v>110</v>
+      </c>
+      <c r="K25" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L25" t="n">
+        <v>59.955</v>
+      </c>
+      <c r="M25" t="n">
+        <v>10.859</v>
+      </c>
+      <c r="N25" t="s">
+        <v>115</v>
+      </c>
+      <c r="O25" t="s">
+        <v>116</v>
+      </c>
+      <c r="P25" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>119</v>
+      </c>
+      <c r="R25" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="S25" t="s">
+        <v>127</v>
+      </c>
+      <c r="T25" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="U25" t="n">
+        <v>25.0</v>
+      </c>
+      <c r="V25" t="s">
+        <v>128</v>
+      </c>
+      <c r="W25" t="s">
+        <v>118</v>
+      </c>
+      <c r="X25" t="s">
+        <v>118</v>
+      </c>
+      <c r="Y25" t="s">
+        <v>155</v>
+      </c>
+      <c r="Z25" t="s">
+        <v>182</v>
+      </c>
+      <c r="AA25" t="s">
+        <v>188</v>
+      </c>
+      <c r="AB25" t="s">
+        <v>213</v>
+      </c>
+      <c r="AC25" t="s">
+        <v>240</v>
+      </c>
+      <c r="AD25" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>53</v>
+      </c>
+      <c r="B26" t="n" s="2">
+        <v>45307.555393518516</v>
+      </c>
+      <c r="C26" t="n" s="2">
+        <v>45307.5608912037</v>
+      </c>
+      <c r="D26" t="s">
+        <v>57</v>
+      </c>
+      <c r="E26" t="s">
+        <v>82</v>
+      </c>
+      <c r="F26" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="G26" t="n">
+        <v>475.0</v>
+      </c>
+      <c r="H26" t="s">
+        <v>86</v>
+      </c>
+      <c r="I26" t="n" s="2">
+        <v>45307.56091435185</v>
+      </c>
+      <c r="J26" t="s">
+        <v>111</v>
+      </c>
+      <c r="K26" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L26" t="n">
+        <v>51.4743</v>
+      </c>
+      <c r="M26" t="n">
+        <v>-0.0928</v>
+      </c>
+      <c r="N26" t="s">
+        <v>115</v>
+      </c>
+      <c r="O26" t="s">
+        <v>116</v>
+      </c>
+      <c r="P26" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>119</v>
+      </c>
+      <c r="R26" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="S26" t="s">
+        <v>127</v>
+      </c>
+      <c r="T26" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="U26" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="V26" t="s">
+        <v>128</v>
+      </c>
+      <c r="W26" t="s">
+        <v>118</v>
+      </c>
+      <c r="X26" t="s">
+        <v>118</v>
+      </c>
+      <c r="Y26" t="s">
+        <v>156</v>
+      </c>
+      <c r="Z26" t="s">
+        <v>183</v>
+      </c>
+      <c r="AA26" t="s">
+        <v>186</v>
+      </c>
+      <c r="AB26" t="s">
+        <v>214</v>
+      </c>
+      <c r="AC26" t="s">
+        <v>241</v>
+      </c>
+      <c r="AD26" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>54</v>
+      </c>
+      <c r="B27" t="n" s="2">
+        <v>45307.88516203704</v>
+      </c>
+      <c r="C27" t="n" s="2">
+        <v>45307.89032407408</v>
+      </c>
+      <c r="D27" t="s">
+        <v>57</v>
+      </c>
+      <c r="E27" t="s">
+        <v>83</v>
+      </c>
+      <c r="F27" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="G27" t="n">
+        <v>445.0</v>
+      </c>
+      <c r="H27" t="s">
+        <v>86</v>
+      </c>
+      <c r="I27" t="n" s="2">
+        <v>45307.890335648146</v>
+      </c>
+      <c r="J27" t="s">
+        <v>112</v>
+      </c>
+      <c r="K27" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L27" t="n">
+        <v>51.9844</v>
+      </c>
+      <c r="M27" t="n">
+        <v>4.1352</v>
+      </c>
+      <c r="N27" t="s">
+        <v>115</v>
+      </c>
+      <c r="O27" t="s">
+        <v>116</v>
+      </c>
+      <c r="P27" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>120</v>
+      </c>
+      <c r="R27" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="S27" t="s">
+        <v>127</v>
+      </c>
+      <c r="T27" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="U27" t="n">
+        <v>35.0</v>
+      </c>
+      <c r="V27" t="s">
+        <v>128</v>
+      </c>
+      <c r="W27" t="s">
+        <v>117</v>
+      </c>
+      <c r="X27" t="s">
+        <v>118</v>
+      </c>
+      <c r="Y27" t="s">
+        <v>157</v>
+      </c>
+      <c r="Z27" t="s">
+        <v>184</v>
+      </c>
+      <c r="AA27" t="s">
+        <v>188</v>
+      </c>
+      <c r="AB27" t="s">
+        <v>215</v>
+      </c>
+      <c r="AC27" t="s">
+        <v>242</v>
+      </c>
+      <c r="AD27" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>55</v>
+      </c>
+      <c r="B28" t="n" s="2">
+        <v>45306.871087962965</v>
+      </c>
+      <c r="C28" t="n" s="2">
+        <v>45308.48578703703</v>
+      </c>
+      <c r="D28" t="s">
+        <v>57</v>
+      </c>
+      <c r="E28" t="s">
+        <v>84</v>
+      </c>
+      <c r="F28" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="G28" t="n">
+        <v>139510.0</v>
+      </c>
+      <c r="H28" t="s">
+        <v>86</v>
+      </c>
+      <c r="I28" t="n" s="2">
+        <v>45308.48579861112</v>
+      </c>
+      <c r="J28" t="s">
+        <v>113</v>
+      </c>
+      <c r="K28" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L28" t="n">
+        <v>52.3441</v>
+      </c>
+      <c r="M28" t="n">
+        <v>4.8782</v>
+      </c>
+      <c r="N28" t="s">
+        <v>115</v>
+      </c>
+      <c r="O28" t="s">
+        <v>116</v>
+      </c>
+      <c r="P28" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q28"/>
+      <c r="R28" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="S28"/>
+      <c r="T28" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="U28" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="V28"/>
+      <c r="W28"/>
+      <c r="X28"/>
+      <c r="Y28" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="Z28" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AA28"/>
+      <c r="AB28" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AC28" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AD28" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>56</v>
+      </c>
+      <c r="B29" t="n" s="2">
+        <v>45308.803888888884</v>
+      </c>
+      <c r="C29" t="n" s="2">
+        <v>45308.823842592596</v>
+      </c>
+      <c r="D29" t="s">
+        <v>57</v>
+      </c>
+      <c r="E29" t="s">
+        <v>85</v>
+      </c>
+      <c r="F29" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="G29" t="n">
+        <v>1723.0</v>
+      </c>
+      <c r="H29" t="s">
+        <v>86</v>
+      </c>
+      <c r="I29" t="n" s="2">
+        <v>45308.82386574074</v>
+      </c>
+      <c r="J29" t="s">
+        <v>114</v>
+      </c>
+      <c r="K29" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L29" t="n">
+        <v>40.7157</v>
+      </c>
+      <c r="M29" t="n">
+        <v>-74.0</v>
+      </c>
+      <c r="N29" t="s">
+        <v>115</v>
+      </c>
+      <c r="O29" t="s">
+        <v>116</v>
+      </c>
+      <c r="P29" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>122</v>
+      </c>
+      <c r="R29" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="S29" t="s">
+        <v>127</v>
+      </c>
+      <c r="T29" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="U29" t="n">
+        <v>28.0</v>
+      </c>
+      <c r="V29" t="s">
+        <v>129</v>
+      </c>
+      <c r="W29" t="s">
+        <v>117</v>
+      </c>
+      <c r="X29" t="s">
+        <v>118</v>
+      </c>
+      <c r="Y29" t="s">
+        <v>158</v>
+      </c>
+      <c r="Z29" t="s">
+        <v>185</v>
+      </c>
+      <c r="AA29" t="s">
+        <v>186</v>
+      </c>
+      <c r="AB29" t="s">
+        <v>216</v>
+      </c>
+      <c r="AC29" t="s">
+        <v>243</v>
+      </c>
+      <c r="AD29" t="s">
+        <v>270</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add report incomplete cases dround 1
</commit_message>
<xml_diff>
--- a/data/clean/Delphi1.xlsx
+++ b/data/clean/Delphi1.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="303">
   <si>
     <t>StartDate</t>
   </si>
@@ -185,6 +185,27 @@
     <t>28</t>
   </si>
   <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>34</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
     <t>IP Address</t>
   </si>
   <si>
@@ -272,9 +293,33 @@
     <t>71.105.254.23</t>
   </si>
   <si>
+    <t>176.169.6.123</t>
+  </si>
+  <si>
+    <t>187.95.189.122</t>
+  </si>
+  <si>
+    <t>141.134.250.181</t>
+  </si>
+  <si>
+    <t>80.106.73.59</t>
+  </si>
+  <si>
+    <t>212.239.158.162</t>
+  </si>
+  <si>
+    <t>131.211.93.86</t>
+  </si>
+  <si>
+    <t>86.89.222.199</t>
+  </si>
+  <si>
     <t>TRUE</t>
   </si>
   <si>
+    <t>FALSE</t>
+  </si>
+  <si>
     <t>R_59bJh7FGjoWuPKt</t>
   </si>
   <si>
@@ -359,6 +404,27 @@
     <t>R_77I1BFSeoy3XnH7</t>
   </si>
   <si>
+    <t>R_1FFat97wyAjbDQe</t>
+  </si>
+  <si>
+    <t>R_1cHJVx1Uh6lWLMB</t>
+  </si>
+  <si>
+    <t>R_2ymtM529VC1vYWY</t>
+  </si>
+  <si>
+    <t>R_2aQ7wNZprR7c8c8</t>
+  </si>
+  <si>
+    <t>R_2lJRCAzmMr6F0yT</t>
+  </si>
+  <si>
+    <t>R_21E43jdVG2YGaWt</t>
+  </si>
+  <si>
+    <t>R_2FTl2qQhZ30XdAd</t>
+  </si>
+  <si>
     <t>email</t>
   </si>
   <si>
@@ -389,6 +455,9 @@
     <t>head of the MHPSS sector of a UN Agency</t>
   </si>
   <si>
+    <t>Humanitarian MH ¨Program Manager</t>
+  </si>
+  <si>
     <t>Mental health</t>
   </si>
   <si>
@@ -408,6 +477,9 @@
   </si>
   <si>
     <t>Asia</t>
+  </si>
+  <si>
+    <t>South America</t>
   </si>
   <si>
     <t>Take care of their own mental health, so that they can remain empathetic.</t>
@@ -574,6 +646,22 @@
     <t>I work with immigrants, refugees and asylum seekers. Most of the asylum seekers I have worked with have been in the context of Mental Health evaluation to support asylum claims, psychotherapy with asylum seekers in hospital and community settings, and training of therapists, and immigration officers in cultural and strucural sensitivity.  In these contexts it is important that the front line workers have education and consultation with a knowledgeable representative (preferably professional) of the culture of the asylum seekers with which one is working.  The transcultural conversations ideally should seek to understand the clients perspective and cultural form of describing distress and its sources, as well as preferred ways of addressing that distress. In addition, what individual, social, cultural resources one needs to draw on to promote psychosocial well-being.</t>
   </si>
   <si>
+    <t>1) Be aware of their own cultural background;
+2) Be open to other cultures;
+3) Be open to alternative explanatory models of "mental illness" and "healing";
+4) Understand the effects of trauma on mental health, and the post-traumatic common reactions;
+5) Have interview skills (e.g., active listening).;</t>
+  </si>
+  <si>
+    <t>must be able to build a solid caregiver relationship in a short period of time before applying solution orientation</t>
+  </si>
+  <si>
+    <t>be aware that: nothing -or quite nothing- is given for granted; people come from completely different backgrounds; many times we may come in contact with them but not meet with them; they may be very cautious towards us since they do not know who we are, which are our intentions and goals; each person is different; only a minority may identify themselves as refugees; they may be disoriented; are very sensitive to perceived uncertainty; we may be all the same to them.</t>
+  </si>
+  <si>
+    <t>Work with a professional interpreter and always get to know the explanatory model of the client. Good mental health care combines the perspective of the mental health sector with the explanatory model of the client. Furthermore, the risk of stigmatisation should be addressed and if possible relatives or friends should be involved, to reduce the risk of stigma and to form a support system</t>
+  </si>
+  <si>
     <t>Psychological first aid</t>
   </si>
   <si>
@@ -670,6 +758,18 @@
   </si>
   <si>
     <t>I participated in the development of the IOM Guidelines for Community based Mental Health and Psychosocial Support in Emergency and Migrant situations. That is a very good source.</t>
+  </si>
+  <si>
+    <t>Cultural formulation interview (CFI; DSM-5)</t>
+  </si>
+  <si>
+    <t>Motivational interviewing</t>
+  </si>
+  <si>
+    <t>the framework coming from the approach of Synergic Therapeutic Complexity (Papadopoulos, RK, 2021, Involuntary Dislocation. Home, Trauma, Resilience and Adversity Activated Development. London. Routledge).</t>
+  </si>
+  <si>
+    <t>no existing framework, but most important guidelines are mentioned above.</t>
   </si>
   <si>
     <t>Probably yes</t>
@@ -1245,10 +1345,10 @@
         <v>45299.34706018519</v>
       </c>
       <c r="D2" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="E2" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="F2" t="n">
         <v>100.0</v>
@@ -1257,13 +1357,13 @@
         <v>270.0</v>
       </c>
       <c r="H2" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="I2" t="n" s="2">
         <v>45299.34707175926</v>
       </c>
       <c r="J2" t="s">
-        <v>87</v>
+        <v>102</v>
       </c>
       <c r="K2" t="e">
         <v>#N/A</v>
@@ -1275,22 +1375,22 @@
         <v>12.5298</v>
       </c>
       <c r="N2" t="s">
-        <v>115</v>
+        <v>137</v>
       </c>
       <c r="O2" t="s">
-        <v>116</v>
+        <v>138</v>
       </c>
       <c r="P2" t="s">
-        <v>117</v>
+        <v>139</v>
       </c>
       <c r="Q2" t="s">
-        <v>119</v>
+        <v>141</v>
       </c>
       <c r="R2" t="e">
         <v>#N/A</v>
       </c>
       <c r="S2" t="s">
-        <v>125</v>
+        <v>148</v>
       </c>
       <c r="T2" t="e">
         <v>#N/A</v>
@@ -1299,31 +1399,31 @@
         <v>15.0</v>
       </c>
       <c r="V2" t="s">
-        <v>128</v>
+        <v>151</v>
       </c>
       <c r="W2" t="s">
-        <v>118</v>
+        <v>140</v>
       </c>
       <c r="X2" t="s">
-        <v>118</v>
+        <v>140</v>
       </c>
       <c r="Y2" t="s">
-        <v>132</v>
+        <v>156</v>
       </c>
       <c r="Z2" t="s">
-        <v>159</v>
+        <v>187</v>
       </c>
       <c r="AA2" t="s">
-        <v>186</v>
+        <v>218</v>
       </c>
       <c r="AB2" t="s">
-        <v>190</v>
+        <v>222</v>
       </c>
       <c r="AC2" t="s">
-        <v>217</v>
+        <v>249</v>
       </c>
       <c r="AD2" t="s">
-        <v>244</v>
+        <v>276</v>
       </c>
     </row>
     <row r="3">
@@ -1337,10 +1437,10 @@
         <v>45299.356840277775</v>
       </c>
       <c r="D3" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="E3" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="F3" t="n">
         <v>100.0</v>
@@ -1349,13 +1449,13 @@
         <v>1822.0</v>
       </c>
       <c r="H3" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="I3" t="n" s="2">
         <v>45299.35685185185</v>
       </c>
       <c r="J3" t="s">
-        <v>88</v>
+        <v>103</v>
       </c>
       <c r="K3" t="e">
         <v>#N/A</v>
@@ -1367,22 +1467,22 @@
         <v>4.9922</v>
       </c>
       <c r="N3" t="s">
-        <v>115</v>
+        <v>137</v>
       </c>
       <c r="O3" t="s">
-        <v>116</v>
+        <v>138</v>
       </c>
       <c r="P3" t="s">
-        <v>117</v>
+        <v>139</v>
       </c>
       <c r="Q3" t="s">
-        <v>119</v>
+        <v>141</v>
       </c>
       <c r="R3" t="e">
         <v>#N/A</v>
       </c>
       <c r="S3" t="s">
-        <v>126</v>
+        <v>149</v>
       </c>
       <c r="T3" t="e">
         <v>#N/A</v>
@@ -1391,31 +1491,31 @@
         <v>17.0</v>
       </c>
       <c r="V3" t="s">
-        <v>128</v>
+        <v>151</v>
       </c>
       <c r="W3" t="s">
-        <v>118</v>
+        <v>140</v>
       </c>
       <c r="X3" t="s">
-        <v>118</v>
+        <v>140</v>
       </c>
       <c r="Y3" t="s">
-        <v>133</v>
+        <v>157</v>
       </c>
       <c r="Z3" t="s">
-        <v>160</v>
+        <v>188</v>
       </c>
       <c r="AA3" t="s">
-        <v>187</v>
+        <v>219</v>
       </c>
       <c r="AB3" t="s">
-        <v>191</v>
+        <v>223</v>
       </c>
       <c r="AC3" t="s">
-        <v>218</v>
+        <v>250</v>
       </c>
       <c r="AD3" t="s">
-        <v>245</v>
+        <v>277</v>
       </c>
     </row>
     <row r="4">
@@ -1429,10 +1529,10 @@
         <v>45299.41439814815</v>
       </c>
       <c r="D4" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="E4" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="F4" t="n">
         <v>100.0</v>
@@ -1441,13 +1541,13 @@
         <v>3842.0</v>
       </c>
       <c r="H4" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="I4" t="n" s="2">
         <v>45299.41440972222</v>
       </c>
       <c r="J4" t="s">
-        <v>89</v>
+        <v>104</v>
       </c>
       <c r="K4" t="e">
         <v>#N/A</v>
@@ -1459,22 +1559,22 @@
         <v>4.7027</v>
       </c>
       <c r="N4" t="s">
-        <v>115</v>
+        <v>137</v>
       </c>
       <c r="O4" t="s">
-        <v>116</v>
+        <v>138</v>
       </c>
       <c r="P4" t="s">
-        <v>117</v>
+        <v>139</v>
       </c>
       <c r="Q4" t="s">
-        <v>120</v>
+        <v>142</v>
       </c>
       <c r="R4" t="e">
         <v>#N/A</v>
       </c>
       <c r="S4" t="s">
-        <v>127</v>
+        <v>150</v>
       </c>
       <c r="T4" t="e">
         <v>#N/A</v>
@@ -1483,31 +1583,31 @@
         <v>20.0</v>
       </c>
       <c r="V4" t="s">
-        <v>128</v>
+        <v>151</v>
       </c>
       <c r="W4" t="s">
-        <v>117</v>
+        <v>139</v>
       </c>
       <c r="X4" t="s">
-        <v>117</v>
+        <v>139</v>
       </c>
       <c r="Y4" t="s">
-        <v>134</v>
+        <v>158</v>
       </c>
       <c r="Z4" t="s">
-        <v>161</v>
+        <v>189</v>
       </c>
       <c r="AA4" t="s">
-        <v>186</v>
+        <v>218</v>
       </c>
       <c r="AB4" t="s">
-        <v>192</v>
+        <v>224</v>
       </c>
       <c r="AC4" t="s">
-        <v>219</v>
+        <v>251</v>
       </c>
       <c r="AD4" t="s">
-        <v>246</v>
+        <v>278</v>
       </c>
     </row>
     <row r="5">
@@ -1521,10 +1621,10 @@
         <v>45299.57168981481</v>
       </c>
       <c r="D5" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="E5" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="F5" t="n">
         <v>100.0</v>
@@ -1533,13 +1633,13 @@
         <v>305.0</v>
       </c>
       <c r="H5" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="I5" t="n" s="2">
         <v>45299.57170138889</v>
       </c>
       <c r="J5" t="s">
-        <v>90</v>
+        <v>105</v>
       </c>
       <c r="K5" t="e">
         <v>#N/A</v>
@@ -1551,22 +1651,22 @@
         <v>-0.0373</v>
       </c>
       <c r="N5" t="s">
-        <v>115</v>
+        <v>137</v>
       </c>
       <c r="O5" t="s">
-        <v>116</v>
+        <v>138</v>
       </c>
       <c r="P5" t="s">
-        <v>117</v>
+        <v>139</v>
       </c>
       <c r="Q5" t="s">
-        <v>120</v>
+        <v>142</v>
       </c>
       <c r="R5" t="e">
         <v>#N/A</v>
       </c>
       <c r="S5" t="s">
-        <v>125</v>
+        <v>148</v>
       </c>
       <c r="T5" t="e">
         <v>#N/A</v>
@@ -1575,31 +1675,31 @@
         <v>20.0</v>
       </c>
       <c r="V5" t="s">
-        <v>128</v>
+        <v>151</v>
       </c>
       <c r="W5" t="s">
-        <v>117</v>
+        <v>139</v>
       </c>
       <c r="X5" t="s">
-        <v>117</v>
+        <v>139</v>
       </c>
       <c r="Y5" t="s">
-        <v>135</v>
+        <v>159</v>
       </c>
       <c r="Z5" t="s">
-        <v>162</v>
+        <v>190</v>
       </c>
       <c r="AA5" t="s">
-        <v>186</v>
+        <v>218</v>
       </c>
       <c r="AB5" t="s">
-        <v>193</v>
+        <v>225</v>
       </c>
       <c r="AC5" t="s">
-        <v>220</v>
+        <v>252</v>
       </c>
       <c r="AD5" t="s">
-        <v>247</v>
+        <v>279</v>
       </c>
     </row>
     <row r="6">
@@ -1613,10 +1713,10 @@
         <v>45299.59695601852</v>
       </c>
       <c r="D6" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="E6" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="F6" t="n">
         <v>100.0</v>
@@ -1625,13 +1725,13 @@
         <v>1150.0</v>
       </c>
       <c r="H6" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="I6" t="n" s="2">
         <v>45299.59697916667</v>
       </c>
       <c r="J6" t="s">
-        <v>91</v>
+        <v>106</v>
       </c>
       <c r="K6" t="e">
         <v>#N/A</v>
@@ -1643,22 +1743,22 @@
         <v>-73.9763</v>
       </c>
       <c r="N6" t="s">
-        <v>115</v>
+        <v>137</v>
       </c>
       <c r="O6" t="s">
-        <v>116</v>
+        <v>138</v>
       </c>
       <c r="P6" t="s">
-        <v>117</v>
+        <v>139</v>
       </c>
       <c r="Q6" t="s">
-        <v>119</v>
+        <v>141</v>
       </c>
       <c r="R6" t="e">
         <v>#N/A</v>
       </c>
       <c r="S6" t="s">
-        <v>126</v>
+        <v>149</v>
       </c>
       <c r="T6" t="e">
         <v>#N/A</v>
@@ -1667,31 +1767,31 @@
         <v>20.0</v>
       </c>
       <c r="V6" t="s">
-        <v>129</v>
+        <v>152</v>
       </c>
       <c r="W6" t="s">
-        <v>118</v>
+        <v>140</v>
       </c>
       <c r="X6" t="s">
-        <v>117</v>
+        <v>139</v>
       </c>
       <c r="Y6" t="s">
-        <v>136</v>
+        <v>160</v>
       </c>
       <c r="Z6" t="s">
-        <v>163</v>
+        <v>191</v>
       </c>
       <c r="AA6" t="s">
-        <v>186</v>
+        <v>218</v>
       </c>
       <c r="AB6" t="s">
-        <v>194</v>
+        <v>226</v>
       </c>
       <c r="AC6" t="s">
-        <v>221</v>
+        <v>253</v>
       </c>
       <c r="AD6" t="s">
-        <v>248</v>
+        <v>280</v>
       </c>
     </row>
     <row r="7">
@@ -1705,10 +1805,10 @@
         <v>45299.68324074074</v>
       </c>
       <c r="D7" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="E7" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="F7" t="n">
         <v>100.0</v>
@@ -1717,13 +1817,13 @@
         <v>489.0</v>
       </c>
       <c r="H7" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="I7" t="n" s="2">
         <v>45299.68325231482</v>
       </c>
       <c r="J7" t="s">
-        <v>92</v>
+        <v>107</v>
       </c>
       <c r="K7" t="e">
         <v>#N/A</v>
@@ -1735,22 +1835,22 @@
         <v>-123.1234</v>
       </c>
       <c r="N7" t="s">
-        <v>115</v>
+        <v>137</v>
       </c>
       <c r="O7" t="s">
-        <v>116</v>
+        <v>138</v>
       </c>
       <c r="P7" t="s">
-        <v>117</v>
+        <v>139</v>
       </c>
       <c r="Q7" t="s">
-        <v>119</v>
+        <v>141</v>
       </c>
       <c r="R7" t="e">
         <v>#N/A</v>
       </c>
       <c r="S7" t="s">
-        <v>127</v>
+        <v>150</v>
       </c>
       <c r="T7" t="e">
         <v>#N/A</v>
@@ -1759,31 +1859,31 @@
         <v>25.0</v>
       </c>
       <c r="V7" t="s">
-        <v>129</v>
+        <v>152</v>
       </c>
       <c r="W7" t="s">
-        <v>117</v>
+        <v>139</v>
       </c>
       <c r="X7" t="s">
-        <v>117</v>
+        <v>139</v>
       </c>
       <c r="Y7" t="s">
-        <v>137</v>
+        <v>161</v>
       </c>
       <c r="Z7" t="s">
-        <v>164</v>
+        <v>192</v>
       </c>
       <c r="AA7" t="s">
-        <v>188</v>
+        <v>220</v>
       </c>
       <c r="AB7" t="s">
-        <v>195</v>
+        <v>227</v>
       </c>
       <c r="AC7" t="s">
-        <v>222</v>
+        <v>254</v>
       </c>
       <c r="AD7" t="s">
-        <v>249</v>
+        <v>281</v>
       </c>
     </row>
     <row r="8">
@@ -1797,10 +1897,10 @@
         <v>45300.07512731482</v>
       </c>
       <c r="D8" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="E8" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="F8" t="n">
         <v>100.0</v>
@@ -1809,13 +1909,13 @@
         <v>45086.0</v>
       </c>
       <c r="H8" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="I8" t="n" s="2">
         <v>45300.07513888889</v>
       </c>
       <c r="J8" t="s">
-        <v>93</v>
+        <v>108</v>
       </c>
       <c r="K8" t="e">
         <v>#N/A</v>
@@ -1827,22 +1927,22 @@
         <v>150.7782</v>
       </c>
       <c r="N8" t="s">
-        <v>115</v>
+        <v>137</v>
       </c>
       <c r="O8" t="s">
-        <v>116</v>
+        <v>138</v>
       </c>
       <c r="P8" t="s">
-        <v>117</v>
+        <v>139</v>
       </c>
       <c r="Q8" t="s">
-        <v>119</v>
+        <v>141</v>
       </c>
       <c r="R8" t="e">
         <v>#N/A</v>
       </c>
       <c r="S8" t="s">
-        <v>125</v>
+        <v>148</v>
       </c>
       <c r="T8" t="e">
         <v>#N/A</v>
@@ -1851,31 +1951,31 @@
         <v>20.0</v>
       </c>
       <c r="V8" t="s">
-        <v>130</v>
+        <v>153</v>
       </c>
       <c r="W8" t="s">
-        <v>117</v>
+        <v>139</v>
       </c>
       <c r="X8" t="s">
-        <v>118</v>
+        <v>140</v>
       </c>
       <c r="Y8" t="s">
-        <v>138</v>
+        <v>162</v>
       </c>
       <c r="Z8" t="s">
-        <v>165</v>
+        <v>193</v>
       </c>
       <c r="AA8" t="s">
-        <v>189</v>
+        <v>221</v>
       </c>
       <c r="AB8" t="s">
-        <v>196</v>
+        <v>228</v>
       </c>
       <c r="AC8" t="s">
-        <v>223</v>
+        <v>255</v>
       </c>
       <c r="AD8" t="s">
-        <v>250</v>
+        <v>282</v>
       </c>
     </row>
     <row r="9">
@@ -1889,10 +1989,10 @@
         <v>45300.39530092593</v>
       </c>
       <c r="D9" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="E9" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="F9" t="n">
         <v>100.0</v>
@@ -1901,13 +2001,13 @@
         <v>805.0</v>
       </c>
       <c r="H9" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="I9" t="n" s="2">
         <v>45300.3953125</v>
       </c>
       <c r="J9" t="s">
-        <v>94</v>
+        <v>109</v>
       </c>
       <c r="K9" t="e">
         <v>#N/A</v>
@@ -1919,22 +2019,22 @@
         <v>5.1907</v>
       </c>
       <c r="N9" t="s">
-        <v>115</v>
+        <v>137</v>
       </c>
       <c r="O9" t="s">
-        <v>116</v>
+        <v>138</v>
       </c>
       <c r="P9" t="s">
-        <v>117</v>
+        <v>139</v>
       </c>
       <c r="Q9" t="s">
-        <v>120</v>
+        <v>142</v>
       </c>
       <c r="R9" t="e">
         <v>#N/A</v>
       </c>
       <c r="S9" t="s">
-        <v>125</v>
+        <v>148</v>
       </c>
       <c r="T9" t="e">
         <v>#N/A</v>
@@ -1943,31 +2043,31 @@
         <v>25.0</v>
       </c>
       <c r="V9" t="s">
-        <v>128</v>
+        <v>151</v>
       </c>
       <c r="W9" t="s">
-        <v>117</v>
+        <v>139</v>
       </c>
       <c r="X9" t="s">
-        <v>118</v>
+        <v>140</v>
       </c>
       <c r="Y9" t="s">
-        <v>139</v>
+        <v>163</v>
       </c>
       <c r="Z9" t="s">
-        <v>166</v>
+        <v>194</v>
       </c>
       <c r="AA9" t="s">
-        <v>189</v>
+        <v>221</v>
       </c>
       <c r="AB9" t="s">
-        <v>197</v>
+        <v>229</v>
       </c>
       <c r="AC9" t="s">
-        <v>224</v>
+        <v>256</v>
       </c>
       <c r="AD9" t="s">
-        <v>251</v>
+        <v>283</v>
       </c>
     </row>
     <row r="10">
@@ -1981,10 +2081,10 @@
         <v>45300.417349537034</v>
       </c>
       <c r="D10" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="E10" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="F10" t="n">
         <v>100.0</v>
@@ -1993,13 +2093,13 @@
         <v>1391.0</v>
       </c>
       <c r="H10" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="I10" t="n" s="2">
         <v>45300.41736111111</v>
       </c>
       <c r="J10" t="s">
-        <v>95</v>
+        <v>110</v>
       </c>
       <c r="K10" t="e">
         <v>#N/A</v>
@@ -2011,22 +2111,22 @@
         <v>4.8777</v>
       </c>
       <c r="N10" t="s">
-        <v>115</v>
+        <v>137</v>
       </c>
       <c r="O10" t="s">
-        <v>116</v>
+        <v>138</v>
       </c>
       <c r="P10" t="s">
-        <v>117</v>
+        <v>139</v>
       </c>
       <c r="Q10" t="s">
-        <v>119</v>
+        <v>141</v>
       </c>
       <c r="R10" t="e">
         <v>#N/A</v>
       </c>
       <c r="S10" t="s">
-        <v>127</v>
+        <v>150</v>
       </c>
       <c r="T10" t="e">
         <v>#N/A</v>
@@ -2035,31 +2135,31 @@
         <v>5.0</v>
       </c>
       <c r="V10" t="s">
-        <v>128</v>
+        <v>151</v>
       </c>
       <c r="W10" t="s">
-        <v>117</v>
+        <v>139</v>
       </c>
       <c r="X10" t="s">
-        <v>118</v>
+        <v>140</v>
       </c>
       <c r="Y10" t="s">
-        <v>140</v>
+        <v>164</v>
       </c>
       <c r="Z10" t="s">
-        <v>167</v>
+        <v>195</v>
       </c>
       <c r="AA10" t="s">
-        <v>186</v>
+        <v>218</v>
       </c>
       <c r="AB10" t="s">
-        <v>198</v>
+        <v>230</v>
       </c>
       <c r="AC10" t="s">
-        <v>225</v>
+        <v>257</v>
       </c>
       <c r="AD10" t="s">
-        <v>252</v>
+        <v>284</v>
       </c>
     </row>
     <row r="11">
@@ -2073,10 +2173,10 @@
         <v>45300.53320601852</v>
       </c>
       <c r="D11" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="E11" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="F11" t="n">
         <v>100.0</v>
@@ -2085,13 +2185,13 @@
         <v>103625.0</v>
       </c>
       <c r="H11" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="I11" t="n" s="2">
         <v>45300.533217592594</v>
       </c>
       <c r="J11" t="s">
-        <v>96</v>
+        <v>111</v>
       </c>
       <c r="K11" t="e">
         <v>#N/A</v>
@@ -2103,22 +2203,22 @@
         <v>4.3356</v>
       </c>
       <c r="N11" t="s">
-        <v>115</v>
+        <v>137</v>
       </c>
       <c r="O11" t="s">
-        <v>116</v>
+        <v>138</v>
       </c>
       <c r="P11" t="s">
-        <v>117</v>
+        <v>139</v>
       </c>
       <c r="Q11" t="s">
-        <v>120</v>
+        <v>142</v>
       </c>
       <c r="R11" t="e">
         <v>#N/A</v>
       </c>
       <c r="S11" t="s">
-        <v>127</v>
+        <v>150</v>
       </c>
       <c r="T11" t="e">
         <v>#N/A</v>
@@ -2127,31 +2227,31 @@
         <v>4.0</v>
       </c>
       <c r="V11" t="s">
-        <v>128</v>
+        <v>151</v>
       </c>
       <c r="W11" t="s">
-        <v>117</v>
+        <v>139</v>
       </c>
       <c r="X11" t="s">
-        <v>118</v>
+        <v>140</v>
       </c>
       <c r="Y11" t="s">
-        <v>141</v>
+        <v>165</v>
       </c>
       <c r="Z11" t="s">
-        <v>168</v>
+        <v>196</v>
       </c>
       <c r="AA11" t="s">
-        <v>186</v>
+        <v>218</v>
       </c>
       <c r="AB11" t="s">
-        <v>199</v>
+        <v>231</v>
       </c>
       <c r="AC11" t="s">
-        <v>226</v>
+        <v>258</v>
       </c>
       <c r="AD11" t="s">
-        <v>253</v>
+        <v>285</v>
       </c>
     </row>
     <row r="12">
@@ -2165,10 +2265,10 @@
         <v>45300.66453703704</v>
       </c>
       <c r="D12" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="E12" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="F12" t="n">
         <v>100.0</v>
@@ -2177,13 +2277,13 @@
         <v>2065.0</v>
       </c>
       <c r="H12" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="I12" t="n" s="2">
         <v>45300.66454861111</v>
       </c>
       <c r="J12" t="s">
-        <v>97</v>
+        <v>112</v>
       </c>
       <c r="K12" t="e">
         <v>#N/A</v>
@@ -2195,22 +2295,22 @@
         <v>-80.843</v>
       </c>
       <c r="N12" t="s">
-        <v>115</v>
+        <v>137</v>
       </c>
       <c r="O12" t="s">
-        <v>116</v>
+        <v>138</v>
       </c>
       <c r="P12" t="s">
-        <v>117</v>
+        <v>139</v>
       </c>
       <c r="Q12" t="s">
-        <v>121</v>
+        <v>143</v>
       </c>
       <c r="R12" t="e">
         <v>#N/A</v>
       </c>
       <c r="S12" t="s">
-        <v>127</v>
+        <v>150</v>
       </c>
       <c r="T12" t="e">
         <v>#N/A</v>
@@ -2219,31 +2319,31 @@
         <v>30.0</v>
       </c>
       <c r="V12" t="s">
-        <v>129</v>
+        <v>152</v>
       </c>
       <c r="W12" t="s">
-        <v>117</v>
+        <v>139</v>
       </c>
       <c r="X12" t="s">
-        <v>117</v>
+        <v>139</v>
       </c>
       <c r="Y12" t="s">
-        <v>142</v>
+        <v>166</v>
       </c>
       <c r="Z12" t="s">
-        <v>169</v>
+        <v>197</v>
       </c>
       <c r="AA12" t="s">
-        <v>186</v>
+        <v>218</v>
       </c>
       <c r="AB12" t="s">
-        <v>200</v>
+        <v>232</v>
       </c>
       <c r="AC12" t="s">
-        <v>227</v>
+        <v>259</v>
       </c>
       <c r="AD12" t="s">
-        <v>254</v>
+        <v>286</v>
       </c>
     </row>
     <row r="13">
@@ -2257,10 +2357,10 @@
         <v>45300.88851851852</v>
       </c>
       <c r="D13" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="E13" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="F13" t="n">
         <v>100.0</v>
@@ -2269,13 +2369,13 @@
         <v>1147.0</v>
       </c>
       <c r="H13" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="I13" t="n" s="2">
         <v>45300.88854166667</v>
       </c>
       <c r="J13" t="s">
-        <v>98</v>
+        <v>113</v>
       </c>
       <c r="K13" t="e">
         <v>#N/A</v>
@@ -2287,22 +2387,22 @@
         <v>5.2577</v>
       </c>
       <c r="N13" t="s">
-        <v>115</v>
+        <v>137</v>
       </c>
       <c r="O13" t="s">
-        <v>116</v>
+        <v>138</v>
       </c>
       <c r="P13" t="s">
-        <v>117</v>
+        <v>139</v>
       </c>
       <c r="Q13" t="s">
-        <v>122</v>
+        <v>144</v>
       </c>
       <c r="R13" t="e">
         <v>#N/A</v>
       </c>
       <c r="S13" t="s">
-        <v>126</v>
+        <v>149</v>
       </c>
       <c r="T13" t="e">
         <v>#N/A</v>
@@ -2311,31 +2411,31 @@
         <v>20.0</v>
       </c>
       <c r="V13" t="s">
-        <v>128</v>
+        <v>151</v>
       </c>
       <c r="W13" t="s">
-        <v>118</v>
+        <v>140</v>
       </c>
       <c r="X13" t="s">
-        <v>118</v>
+        <v>140</v>
       </c>
       <c r="Y13" t="s">
-        <v>143</v>
+        <v>167</v>
       </c>
       <c r="Z13" t="s">
-        <v>170</v>
+        <v>198</v>
       </c>
       <c r="AA13" t="s">
-        <v>186</v>
+        <v>218</v>
       </c>
       <c r="AB13" t="s">
-        <v>201</v>
+        <v>233</v>
       </c>
       <c r="AC13" t="s">
-        <v>228</v>
+        <v>260</v>
       </c>
       <c r="AD13" t="s">
-        <v>255</v>
+        <v>287</v>
       </c>
     </row>
     <row r="14">
@@ -2349,10 +2449,10 @@
         <v>45301.86099537037</v>
       </c>
       <c r="D14" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="E14" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="F14" t="n">
         <v>100.0</v>
@@ -2361,13 +2461,13 @@
         <v>69113.0</v>
       </c>
       <c r="H14" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="I14" t="n" s="2">
         <v>45301.86100694444</v>
       </c>
       <c r="J14" t="s">
-        <v>99</v>
+        <v>114</v>
       </c>
       <c r="K14" t="e">
         <v>#N/A</v>
@@ -2379,22 +2479,22 @@
         <v>-77.5546</v>
       </c>
       <c r="N14" t="s">
-        <v>115</v>
+        <v>137</v>
       </c>
       <c r="O14" t="s">
-        <v>116</v>
+        <v>138</v>
       </c>
       <c r="P14" t="s">
-        <v>117</v>
+        <v>139</v>
       </c>
       <c r="Q14" t="s">
-        <v>119</v>
+        <v>141</v>
       </c>
       <c r="R14" t="e">
         <v>#N/A</v>
       </c>
       <c r="S14" t="s">
-        <v>127</v>
+        <v>150</v>
       </c>
       <c r="T14" t="e">
         <v>#N/A</v>
@@ -2403,31 +2503,31 @@
         <v>21.0</v>
       </c>
       <c r="V14" t="s">
-        <v>129</v>
+        <v>152</v>
       </c>
       <c r="W14" t="s">
-        <v>117</v>
+        <v>139</v>
       </c>
       <c r="X14" t="s">
-        <v>118</v>
+        <v>140</v>
       </c>
       <c r="Y14" t="s">
-        <v>144</v>
+        <v>168</v>
       </c>
       <c r="Z14" t="s">
-        <v>171</v>
+        <v>199</v>
       </c>
       <c r="AA14" t="s">
-        <v>189</v>
+        <v>221</v>
       </c>
       <c r="AB14" t="s">
-        <v>202</v>
+        <v>234</v>
       </c>
       <c r="AC14" t="s">
-        <v>229</v>
+        <v>261</v>
       </c>
       <c r="AD14" t="s">
-        <v>256</v>
+        <v>288</v>
       </c>
     </row>
     <row r="15">
@@ -2441,10 +2541,10 @@
         <v>45303.72300925926</v>
       </c>
       <c r="D15" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="E15" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="F15" t="n">
         <v>100.0</v>
@@ -2453,13 +2553,13 @@
         <v>957.0</v>
       </c>
       <c r="H15" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="I15" t="n" s="2">
         <v>45303.723020833335</v>
       </c>
       <c r="J15" t="s">
-        <v>100</v>
+        <v>115</v>
       </c>
       <c r="K15" t="e">
         <v>#N/A</v>
@@ -2471,22 +2571,22 @@
         <v>18.0517</v>
       </c>
       <c r="N15" t="s">
-        <v>115</v>
+        <v>137</v>
       </c>
       <c r="O15" t="s">
-        <v>116</v>
+        <v>138</v>
       </c>
       <c r="P15" t="s">
-        <v>117</v>
+        <v>139</v>
       </c>
       <c r="Q15" t="s">
-        <v>119</v>
+        <v>141</v>
       </c>
       <c r="R15" t="e">
         <v>#N/A</v>
       </c>
       <c r="S15" t="s">
-        <v>127</v>
+        <v>150</v>
       </c>
       <c r="T15" t="e">
         <v>#N/A</v>
@@ -2495,31 +2595,31 @@
         <v>30.0</v>
       </c>
       <c r="V15" t="s">
-        <v>128</v>
+        <v>151</v>
       </c>
       <c r="W15" t="s">
-        <v>117</v>
+        <v>139</v>
       </c>
       <c r="X15" t="s">
-        <v>117</v>
+        <v>139</v>
       </c>
       <c r="Y15" t="s">
-        <v>145</v>
+        <v>169</v>
       </c>
       <c r="Z15" t="s">
-        <v>172</v>
+        <v>200</v>
       </c>
       <c r="AA15" t="s">
-        <v>188</v>
+        <v>220</v>
       </c>
       <c r="AB15" t="s">
-        <v>203</v>
+        <v>235</v>
       </c>
       <c r="AC15" t="s">
-        <v>230</v>
+        <v>262</v>
       </c>
       <c r="AD15" t="s">
-        <v>257</v>
+        <v>289</v>
       </c>
     </row>
     <row r="16">
@@ -2533,10 +2633,10 @@
         <v>45304.01983796296</v>
       </c>
       <c r="D16" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="E16" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="F16" t="n">
         <v>100.0</v>
@@ -2545,13 +2645,13 @@
         <v>3389.0</v>
       </c>
       <c r="H16" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="I16" t="n" s="2">
         <v>45304.01984953704</v>
       </c>
       <c r="J16" t="s">
-        <v>101</v>
+        <v>116</v>
       </c>
       <c r="K16" t="e">
         <v>#N/A</v>
@@ -2563,22 +2663,22 @@
         <v>-79.188</v>
       </c>
       <c r="N16" t="s">
-        <v>115</v>
+        <v>137</v>
       </c>
       <c r="O16" t="s">
-        <v>116</v>
+        <v>138</v>
       </c>
       <c r="P16" t="s">
-        <v>117</v>
+        <v>139</v>
       </c>
       <c r="Q16" t="s">
-        <v>120</v>
+        <v>142</v>
       </c>
       <c r="R16" t="e">
         <v>#N/A</v>
       </c>
       <c r="S16" t="s">
-        <v>127</v>
+        <v>150</v>
       </c>
       <c r="T16" t="e">
         <v>#N/A</v>
@@ -2587,31 +2687,31 @@
         <v>30.0</v>
       </c>
       <c r="V16" t="s">
-        <v>129</v>
+        <v>152</v>
       </c>
       <c r="W16" t="s">
-        <v>117</v>
+        <v>139</v>
       </c>
       <c r="X16" t="s">
-        <v>118</v>
+        <v>140</v>
       </c>
       <c r="Y16" t="s">
-        <v>146</v>
+        <v>170</v>
       </c>
       <c r="Z16" t="s">
-        <v>173</v>
+        <v>201</v>
       </c>
       <c r="AA16" t="s">
-        <v>186</v>
+        <v>218</v>
       </c>
       <c r="AB16" t="s">
-        <v>204</v>
+        <v>236</v>
       </c>
       <c r="AC16" t="s">
-        <v>231</v>
+        <v>263</v>
       </c>
       <c r="AD16" t="s">
-        <v>258</v>
+        <v>290</v>
       </c>
     </row>
     <row r="17">
@@ -2625,10 +2725,10 @@
         <v>45306.346180555556</v>
       </c>
       <c r="D17" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="E17" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="F17" t="n">
         <v>100.0</v>
@@ -2637,13 +2737,13 @@
         <v>4101.0</v>
       </c>
       <c r="H17" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="I17" t="n" s="2">
         <v>45306.346192129626</v>
       </c>
       <c r="J17" t="s">
-        <v>102</v>
+        <v>117</v>
       </c>
       <c r="K17" t="e">
         <v>#N/A</v>
@@ -2655,22 +2755,22 @@
         <v>51.5321</v>
       </c>
       <c r="N17" t="s">
-        <v>115</v>
+        <v>137</v>
       </c>
       <c r="O17" t="s">
-        <v>116</v>
+        <v>138</v>
       </c>
       <c r="P17" t="s">
-        <v>117</v>
+        <v>139</v>
       </c>
       <c r="Q17" t="s">
-        <v>121</v>
+        <v>143</v>
       </c>
       <c r="R17" t="e">
         <v>#N/A</v>
       </c>
       <c r="S17" t="s">
-        <v>125</v>
+        <v>148</v>
       </c>
       <c r="T17" t="e">
         <v>#N/A</v>
@@ -2679,31 +2779,31 @@
         <v>26.0</v>
       </c>
       <c r="V17" t="s">
-        <v>130</v>
+        <v>153</v>
       </c>
       <c r="W17" t="s">
-        <v>117</v>
+        <v>139</v>
       </c>
       <c r="X17" t="s">
-        <v>117</v>
+        <v>139</v>
       </c>
       <c r="Y17" t="s">
-        <v>147</v>
+        <v>171</v>
       </c>
       <c r="Z17" t="s">
-        <v>174</v>
+        <v>202</v>
       </c>
       <c r="AA17" t="s">
-        <v>189</v>
+        <v>221</v>
       </c>
       <c r="AB17" t="s">
-        <v>205</v>
+        <v>237</v>
       </c>
       <c r="AC17" t="s">
-        <v>232</v>
+        <v>264</v>
       </c>
       <c r="AD17" t="s">
-        <v>259</v>
+        <v>291</v>
       </c>
     </row>
     <row r="18">
@@ -2717,10 +2817,10 @@
         <v>45306.36274305556</v>
       </c>
       <c r="D18" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="E18" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="F18" t="n">
         <v>100.0</v>
@@ -2729,13 +2829,13 @@
         <v>600161.0</v>
       </c>
       <c r="H18" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="I18" t="n" s="2">
         <v>45306.362754629634</v>
       </c>
       <c r="J18" t="s">
-        <v>103</v>
+        <v>118</v>
       </c>
       <c r="K18" t="e">
         <v>#N/A</v>
@@ -2747,22 +2847,22 @@
         <v>8.5671</v>
       </c>
       <c r="N18" t="s">
-        <v>115</v>
+        <v>137</v>
       </c>
       <c r="O18" t="s">
-        <v>116</v>
+        <v>138</v>
       </c>
       <c r="P18" t="s">
-        <v>117</v>
+        <v>139</v>
       </c>
       <c r="Q18" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="R18" t="s">
-        <v>124</v>
+        <v>146</v>
       </c>
       <c r="S18" t="s">
-        <v>127</v>
+        <v>150</v>
       </c>
       <c r="T18" t="e">
         <v>#N/A</v>
@@ -2771,31 +2871,31 @@
         <v>22.0</v>
       </c>
       <c r="V18" t="s">
-        <v>128</v>
+        <v>151</v>
       </c>
       <c r="W18" t="s">
-        <v>117</v>
+        <v>139</v>
       </c>
       <c r="X18" t="s">
-        <v>117</v>
+        <v>139</v>
       </c>
       <c r="Y18" t="s">
-        <v>148</v>
+        <v>172</v>
       </c>
       <c r="Z18" t="s">
-        <v>175</v>
+        <v>203</v>
       </c>
       <c r="AA18" t="s">
-        <v>188</v>
+        <v>220</v>
       </c>
       <c r="AB18" t="s">
-        <v>206</v>
+        <v>238</v>
       </c>
       <c r="AC18" t="s">
-        <v>233</v>
+        <v>265</v>
       </c>
       <c r="AD18" t="s">
-        <v>260</v>
+        <v>292</v>
       </c>
     </row>
     <row r="19">
@@ -2809,10 +2909,10 @@
         <v>45306.40620370371</v>
       </c>
       <c r="D19" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="E19" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="F19" t="n">
         <v>100.0</v>
@@ -2821,13 +2921,13 @@
         <v>960.0</v>
       </c>
       <c r="H19" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="I19" t="n" s="2">
         <v>45306.40621527778</v>
       </c>
       <c r="J19" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
       <c r="K19" t="e">
         <v>#N/A</v>
@@ -2839,22 +2939,22 @@
         <v>-0.066</v>
       </c>
       <c r="N19" t="s">
-        <v>115</v>
+        <v>137</v>
       </c>
       <c r="O19" t="s">
-        <v>116</v>
+        <v>138</v>
       </c>
       <c r="P19" t="s">
-        <v>117</v>
+        <v>139</v>
       </c>
       <c r="Q19" t="s">
-        <v>120</v>
+        <v>142</v>
       </c>
       <c r="R19" t="e">
         <v>#N/A</v>
       </c>
       <c r="S19" t="s">
-        <v>125</v>
+        <v>148</v>
       </c>
       <c r="T19" t="e">
         <v>#N/A</v>
@@ -2863,31 +2963,31 @@
         <v>15.0</v>
       </c>
       <c r="V19" t="s">
-        <v>131</v>
+        <v>154</v>
       </c>
       <c r="W19" t="s">
-        <v>117</v>
+        <v>139</v>
       </c>
       <c r="X19" t="s">
-        <v>118</v>
+        <v>140</v>
       </c>
       <c r="Y19" t="s">
-        <v>149</v>
+        <v>173</v>
       </c>
       <c r="Z19" t="s">
-        <v>176</v>
+        <v>204</v>
       </c>
       <c r="AA19" t="s">
-        <v>186</v>
+        <v>218</v>
       </c>
       <c r="AB19" t="s">
-        <v>207</v>
+        <v>239</v>
       </c>
       <c r="AC19" t="s">
-        <v>234</v>
+        <v>266</v>
       </c>
       <c r="AD19" t="s">
-        <v>261</v>
+        <v>293</v>
       </c>
     </row>
     <row r="20">
@@ -2901,10 +3001,10 @@
         <v>45306.474270833336</v>
       </c>
       <c r="D20" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="E20" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="F20" t="n">
         <v>100.0</v>
@@ -2913,13 +3013,13 @@
         <v>8378.0</v>
       </c>
       <c r="H20" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="I20" t="n" s="2">
         <v>45306.474282407406</v>
       </c>
       <c r="J20" t="s">
-        <v>105</v>
+        <v>120</v>
       </c>
       <c r="K20" t="e">
         <v>#N/A</v>
@@ -2931,22 +3031,22 @@
         <v>-0.1235</v>
       </c>
       <c r="N20" t="s">
-        <v>115</v>
+        <v>137</v>
       </c>
       <c r="O20" t="s">
-        <v>116</v>
+        <v>138</v>
       </c>
       <c r="P20" t="s">
-        <v>117</v>
+        <v>139</v>
       </c>
       <c r="Q20" t="s">
-        <v>120</v>
+        <v>142</v>
       </c>
       <c r="R20" t="e">
         <v>#N/A</v>
       </c>
       <c r="S20" t="s">
-        <v>125</v>
+        <v>148</v>
       </c>
       <c r="T20" t="e">
         <v>#N/A</v>
@@ -2955,31 +3055,31 @@
         <v>20.0</v>
       </c>
       <c r="V20" t="s">
-        <v>128</v>
+        <v>151</v>
       </c>
       <c r="W20" t="s">
-        <v>117</v>
+        <v>139</v>
       </c>
       <c r="X20" t="s">
-        <v>118</v>
+        <v>140</v>
       </c>
       <c r="Y20" t="s">
-        <v>150</v>
+        <v>174</v>
       </c>
       <c r="Z20" t="s">
-        <v>177</v>
+        <v>205</v>
       </c>
       <c r="AA20" t="s">
-        <v>188</v>
+        <v>220</v>
       </c>
       <c r="AB20" t="s">
-        <v>208</v>
+        <v>240</v>
       </c>
       <c r="AC20" t="s">
-        <v>235</v>
+        <v>267</v>
       </c>
       <c r="AD20" t="s">
-        <v>262</v>
+        <v>294</v>
       </c>
     </row>
     <row r="21">
@@ -2993,10 +3093,10 @@
         <v>45306.49673611111</v>
       </c>
       <c r="D21" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="E21" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="F21" t="n">
         <v>100.0</v>
@@ -3005,13 +3105,13 @@
         <v>633.0</v>
       </c>
       <c r="H21" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="I21" t="n" s="2">
         <v>45306.49674768519</v>
       </c>
       <c r="J21" t="s">
-        <v>106</v>
+        <v>121</v>
       </c>
       <c r="K21" t="e">
         <v>#N/A</v>
@@ -3023,22 +3123,22 @@
         <v>5.3275</v>
       </c>
       <c r="N21" t="s">
-        <v>115</v>
+        <v>137</v>
       </c>
       <c r="O21" t="s">
-        <v>116</v>
+        <v>138</v>
       </c>
       <c r="P21" t="s">
-        <v>117</v>
+        <v>139</v>
       </c>
       <c r="Q21" t="s">
-        <v>119</v>
+        <v>141</v>
       </c>
       <c r="R21" t="e">
         <v>#N/A</v>
       </c>
       <c r="S21" t="s">
-        <v>127</v>
+        <v>150</v>
       </c>
       <c r="T21" t="e">
         <v>#N/A</v>
@@ -3047,31 +3147,31 @@
         <v>7.0</v>
       </c>
       <c r="V21" t="s">
-        <v>128</v>
+        <v>151</v>
       </c>
       <c r="W21" t="s">
-        <v>117</v>
+        <v>139</v>
       </c>
       <c r="X21" t="s">
-        <v>118</v>
+        <v>140</v>
       </c>
       <c r="Y21" t="s">
-        <v>151</v>
+        <v>175</v>
       </c>
       <c r="Z21" t="s">
-        <v>178</v>
+        <v>206</v>
       </c>
       <c r="AA21" t="s">
-        <v>186</v>
+        <v>218</v>
       </c>
       <c r="AB21" t="s">
-        <v>209</v>
+        <v>241</v>
       </c>
       <c r="AC21" t="s">
-        <v>236</v>
+        <v>268</v>
       </c>
       <c r="AD21" t="s">
-        <v>263</v>
+        <v>295</v>
       </c>
     </row>
     <row r="22">
@@ -3085,10 +3185,10 @@
         <v>45306.67015046296</v>
       </c>
       <c r="D22" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="E22" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="F22" t="n">
         <v>100.0</v>
@@ -3097,13 +3197,13 @@
         <v>14159.0</v>
       </c>
       <c r="H22" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="I22" t="n" s="2">
         <v>45306.67016203704</v>
       </c>
       <c r="J22" t="s">
-        <v>107</v>
+        <v>122</v>
       </c>
       <c r="K22" t="e">
         <v>#N/A</v>
@@ -3115,22 +3215,22 @@
         <v>-0.0096</v>
       </c>
       <c r="N22" t="s">
-        <v>115</v>
+        <v>137</v>
       </c>
       <c r="O22" t="s">
-        <v>116</v>
+        <v>138</v>
       </c>
       <c r="P22" t="s">
-        <v>117</v>
+        <v>139</v>
       </c>
       <c r="Q22" t="s">
-        <v>119</v>
+        <v>141</v>
       </c>
       <c r="R22" t="e">
         <v>#N/A</v>
       </c>
       <c r="S22" t="s">
-        <v>125</v>
+        <v>148</v>
       </c>
       <c r="T22" t="e">
         <v>#N/A</v>
@@ -3139,31 +3239,31 @@
         <v>40.0</v>
       </c>
       <c r="V22" t="s">
-        <v>128</v>
+        <v>151</v>
       </c>
       <c r="W22" t="s">
-        <v>118</v>
+        <v>140</v>
       </c>
       <c r="X22" t="s">
-        <v>118</v>
+        <v>140</v>
       </c>
       <c r="Y22" t="s">
-        <v>152</v>
+        <v>176</v>
       </c>
       <c r="Z22" t="s">
-        <v>179</v>
+        <v>207</v>
       </c>
       <c r="AA22" t="s">
-        <v>188</v>
+        <v>220</v>
       </c>
       <c r="AB22" t="s">
-        <v>210</v>
+        <v>242</v>
       </c>
       <c r="AC22" t="s">
-        <v>237</v>
+        <v>269</v>
       </c>
       <c r="AD22" t="s">
-        <v>264</v>
+        <v>296</v>
       </c>
     </row>
     <row r="23">
@@ -3177,10 +3277,10 @@
         <v>45306.826828703706</v>
       </c>
       <c r="D23" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="E23" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="F23" t="n">
         <v>100.0</v>
@@ -3189,13 +3289,13 @@
         <v>291.0</v>
       </c>
       <c r="H23" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="I23" t="n" s="2">
         <v>45306.826840277776</v>
       </c>
       <c r="J23" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
       <c r="K23" t="e">
         <v>#N/A</v>
@@ -3207,22 +3307,22 @@
         <v>-16.9</v>
       </c>
       <c r="N23" t="s">
-        <v>115</v>
+        <v>137</v>
       </c>
       <c r="O23" t="s">
-        <v>116</v>
+        <v>138</v>
       </c>
       <c r="P23" t="s">
-        <v>117</v>
+        <v>139</v>
       </c>
       <c r="Q23" t="s">
-        <v>119</v>
+        <v>141</v>
       </c>
       <c r="R23" t="e">
         <v>#N/A</v>
       </c>
       <c r="S23" t="s">
-        <v>127</v>
+        <v>150</v>
       </c>
       <c r="T23" t="e">
         <v>#N/A</v>
@@ -3231,31 +3331,31 @@
         <v>22.0</v>
       </c>
       <c r="V23" t="s">
-        <v>128</v>
+        <v>151</v>
       </c>
       <c r="W23" t="s">
-        <v>118</v>
+        <v>140</v>
       </c>
       <c r="X23" t="s">
-        <v>117</v>
+        <v>139</v>
       </c>
       <c r="Y23" t="s">
-        <v>153</v>
+        <v>177</v>
       </c>
       <c r="Z23" t="s">
-        <v>180</v>
+        <v>208</v>
       </c>
       <c r="AA23" t="s">
-        <v>188</v>
+        <v>220</v>
       </c>
       <c r="AB23" t="s">
-        <v>211</v>
+        <v>243</v>
       </c>
       <c r="AC23" t="s">
-        <v>238</v>
+        <v>270</v>
       </c>
       <c r="AD23" t="s">
-        <v>265</v>
+        <v>297</v>
       </c>
     </row>
     <row r="24">
@@ -3269,10 +3369,10 @@
         <v>45307.27956018518</v>
       </c>
       <c r="D24" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="E24" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="F24" t="n">
         <v>100.0</v>
@@ -3281,13 +3381,13 @@
         <v>747.0</v>
       </c>
       <c r="H24" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="I24" t="n" s="2">
         <v>45307.27957175926</v>
       </c>
       <c r="J24" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
       <c r="K24" t="e">
         <v>#N/A</v>
@@ -3299,22 +3399,22 @@
         <v>-0.0247</v>
       </c>
       <c r="N24" t="s">
-        <v>115</v>
+        <v>137</v>
       </c>
       <c r="O24" t="s">
-        <v>116</v>
+        <v>138</v>
       </c>
       <c r="P24" t="s">
-        <v>117</v>
+        <v>139</v>
       </c>
       <c r="Q24" t="s">
-        <v>121</v>
+        <v>143</v>
       </c>
       <c r="R24" t="e">
         <v>#N/A</v>
       </c>
       <c r="S24" t="s">
-        <v>127</v>
+        <v>150</v>
       </c>
       <c r="T24" t="e">
         <v>#N/A</v>
@@ -3323,31 +3423,31 @@
         <v>20.0</v>
       </c>
       <c r="V24" t="s">
-        <v>128</v>
+        <v>151</v>
       </c>
       <c r="W24" t="s">
-        <v>117</v>
+        <v>139</v>
       </c>
       <c r="X24" t="s">
-        <v>118</v>
+        <v>140</v>
       </c>
       <c r="Y24" t="s">
-        <v>154</v>
+        <v>178</v>
       </c>
       <c r="Z24" t="s">
-        <v>181</v>
+        <v>209</v>
       </c>
       <c r="AA24" t="s">
-        <v>186</v>
+        <v>218</v>
       </c>
       <c r="AB24" t="s">
-        <v>212</v>
+        <v>244</v>
       </c>
       <c r="AC24" t="s">
-        <v>239</v>
+        <v>271</v>
       </c>
       <c r="AD24" t="s">
-        <v>266</v>
+        <v>298</v>
       </c>
     </row>
     <row r="25">
@@ -3361,10 +3461,10 @@
         <v>45307.4065625</v>
       </c>
       <c r="D25" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="E25" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="F25" t="n">
         <v>100.0</v>
@@ -3373,13 +3473,13 @@
         <v>5942.0</v>
       </c>
       <c r="H25" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="I25" t="n" s="2">
         <v>45307.40657407408</v>
       </c>
       <c r="J25" t="s">
-        <v>110</v>
+        <v>125</v>
       </c>
       <c r="K25" t="e">
         <v>#N/A</v>
@@ -3391,22 +3491,22 @@
         <v>10.859</v>
       </c>
       <c r="N25" t="s">
-        <v>115</v>
+        <v>137</v>
       </c>
       <c r="O25" t="s">
-        <v>116</v>
+        <v>138</v>
       </c>
       <c r="P25" t="s">
-        <v>117</v>
+        <v>139</v>
       </c>
       <c r="Q25" t="s">
-        <v>119</v>
+        <v>141</v>
       </c>
       <c r="R25" t="e">
         <v>#N/A</v>
       </c>
       <c r="S25" t="s">
-        <v>127</v>
+        <v>150</v>
       </c>
       <c r="T25" t="e">
         <v>#N/A</v>
@@ -3415,31 +3515,31 @@
         <v>25.0</v>
       </c>
       <c r="V25" t="s">
-        <v>128</v>
+        <v>151</v>
       </c>
       <c r="W25" t="s">
-        <v>118</v>
+        <v>140</v>
       </c>
       <c r="X25" t="s">
-        <v>118</v>
+        <v>140</v>
       </c>
       <c r="Y25" t="s">
-        <v>155</v>
+        <v>179</v>
       </c>
       <c r="Z25" t="s">
-        <v>182</v>
+        <v>210</v>
       </c>
       <c r="AA25" t="s">
-        <v>188</v>
+        <v>220</v>
       </c>
       <c r="AB25" t="s">
-        <v>213</v>
+        <v>245</v>
       </c>
       <c r="AC25" t="s">
-        <v>240</v>
+        <v>272</v>
       </c>
       <c r="AD25" t="s">
-        <v>267</v>
+        <v>299</v>
       </c>
     </row>
     <row r="26">
@@ -3453,10 +3553,10 @@
         <v>45307.5608912037</v>
       </c>
       <c r="D26" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="E26" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="F26" t="n">
         <v>100.0</v>
@@ -3465,13 +3565,13 @@
         <v>475.0</v>
       </c>
       <c r="H26" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="I26" t="n" s="2">
         <v>45307.56091435185</v>
       </c>
       <c r="J26" t="s">
-        <v>111</v>
+        <v>126</v>
       </c>
       <c r="K26" t="e">
         <v>#N/A</v>
@@ -3483,22 +3583,22 @@
         <v>-0.0928</v>
       </c>
       <c r="N26" t="s">
-        <v>115</v>
+        <v>137</v>
       </c>
       <c r="O26" t="s">
-        <v>116</v>
+        <v>138</v>
       </c>
       <c r="P26" t="s">
-        <v>117</v>
+        <v>139</v>
       </c>
       <c r="Q26" t="s">
-        <v>119</v>
+        <v>141</v>
       </c>
       <c r="R26" t="e">
         <v>#N/A</v>
       </c>
       <c r="S26" t="s">
-        <v>127</v>
+        <v>150</v>
       </c>
       <c r="T26" t="e">
         <v>#N/A</v>
@@ -3507,31 +3607,31 @@
         <v>10.0</v>
       </c>
       <c r="V26" t="s">
-        <v>128</v>
+        <v>151</v>
       </c>
       <c r="W26" t="s">
-        <v>118</v>
+        <v>140</v>
       </c>
       <c r="X26" t="s">
-        <v>118</v>
+        <v>140</v>
       </c>
       <c r="Y26" t="s">
-        <v>156</v>
+        <v>180</v>
       </c>
       <c r="Z26" t="s">
-        <v>183</v>
+        <v>211</v>
       </c>
       <c r="AA26" t="s">
-        <v>186</v>
+        <v>218</v>
       </c>
       <c r="AB26" t="s">
-        <v>214</v>
+        <v>246</v>
       </c>
       <c r="AC26" t="s">
-        <v>241</v>
+        <v>273</v>
       </c>
       <c r="AD26" t="s">
-        <v>268</v>
+        <v>300</v>
       </c>
     </row>
     <row r="27">
@@ -3545,10 +3645,10 @@
         <v>45307.89032407408</v>
       </c>
       <c r="D27" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="E27" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="F27" t="n">
         <v>100.0</v>
@@ -3557,13 +3657,13 @@
         <v>445.0</v>
       </c>
       <c r="H27" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="I27" t="n" s="2">
         <v>45307.890335648146</v>
       </c>
       <c r="J27" t="s">
-        <v>112</v>
+        <v>127</v>
       </c>
       <c r="K27" t="e">
         <v>#N/A</v>
@@ -3575,22 +3675,22 @@
         <v>4.1352</v>
       </c>
       <c r="N27" t="s">
-        <v>115</v>
+        <v>137</v>
       </c>
       <c r="O27" t="s">
-        <v>116</v>
+        <v>138</v>
       </c>
       <c r="P27" t="s">
-        <v>117</v>
+        <v>139</v>
       </c>
       <c r="Q27" t="s">
-        <v>120</v>
+        <v>142</v>
       </c>
       <c r="R27" t="e">
         <v>#N/A</v>
       </c>
       <c r="S27" t="s">
-        <v>127</v>
+        <v>150</v>
       </c>
       <c r="T27" t="e">
         <v>#N/A</v>
@@ -3599,31 +3699,31 @@
         <v>35.0</v>
       </c>
       <c r="V27" t="s">
-        <v>128</v>
+        <v>151</v>
       </c>
       <c r="W27" t="s">
-        <v>117</v>
+        <v>139</v>
       </c>
       <c r="X27" t="s">
-        <v>118</v>
+        <v>140</v>
       </c>
       <c r="Y27" t="s">
-        <v>157</v>
+        <v>181</v>
       </c>
       <c r="Z27" t="s">
-        <v>184</v>
+        <v>212</v>
       </c>
       <c r="AA27" t="s">
-        <v>188</v>
+        <v>220</v>
       </c>
       <c r="AB27" t="s">
-        <v>215</v>
+        <v>247</v>
       </c>
       <c r="AC27" t="s">
-        <v>242</v>
+        <v>274</v>
       </c>
       <c r="AD27" t="s">
-        <v>269</v>
+        <v>301</v>
       </c>
     </row>
     <row r="28">
@@ -3637,10 +3737,10 @@
         <v>45308.48578703703</v>
       </c>
       <c r="D28" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="E28" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="F28" t="n">
         <v>100.0</v>
@@ -3649,13 +3749,13 @@
         <v>139510.0</v>
       </c>
       <c r="H28" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="I28" t="n" s="2">
         <v>45308.48579861112</v>
       </c>
       <c r="J28" t="s">
-        <v>113</v>
+        <v>128</v>
       </c>
       <c r="K28" t="e">
         <v>#N/A</v>
@@ -3667,13 +3767,13 @@
         <v>4.8782</v>
       </c>
       <c r="N28" t="s">
-        <v>115</v>
+        <v>137</v>
       </c>
       <c r="O28" t="s">
-        <v>116</v>
+        <v>138</v>
       </c>
       <c r="P28" t="s">
-        <v>118</v>
+        <v>140</v>
       </c>
       <c r="Q28"/>
       <c r="R28" t="e">
@@ -3717,10 +3817,10 @@
         <v>45308.823842592596</v>
       </c>
       <c r="D29" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="E29" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="F29" t="n">
         <v>100.0</v>
@@ -3729,13 +3829,13 @@
         <v>1723.0</v>
       </c>
       <c r="H29" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="I29" t="n" s="2">
         <v>45308.82386574074</v>
       </c>
       <c r="J29" t="s">
-        <v>114</v>
+        <v>129</v>
       </c>
       <c r="K29" t="e">
         <v>#N/A</v>
@@ -3747,22 +3847,22 @@
         <v>-74.0</v>
       </c>
       <c r="N29" t="s">
-        <v>115</v>
+        <v>137</v>
       </c>
       <c r="O29" t="s">
-        <v>116</v>
+        <v>138</v>
       </c>
       <c r="P29" t="s">
-        <v>117</v>
+        <v>139</v>
       </c>
       <c r="Q29" t="s">
-        <v>122</v>
+        <v>144</v>
       </c>
       <c r="R29" t="e">
         <v>#N/A</v>
       </c>
       <c r="S29" t="s">
-        <v>127</v>
+        <v>150</v>
       </c>
       <c r="T29" t="e">
         <v>#N/A</v>
@@ -3771,31 +3871,669 @@
         <v>28.0</v>
       </c>
       <c r="V29" t="s">
-        <v>129</v>
+        <v>152</v>
       </c>
       <c r="W29" t="s">
-        <v>117</v>
+        <v>139</v>
       </c>
       <c r="X29" t="s">
-        <v>118</v>
+        <v>140</v>
       </c>
       <c r="Y29" t="s">
-        <v>158</v>
+        <v>182</v>
       </c>
       <c r="Z29" t="s">
+        <v>213</v>
+      </c>
+      <c r="AA29" t="s">
+        <v>218</v>
+      </c>
+      <c r="AB29" t="s">
+        <v>248</v>
+      </c>
+      <c r="AC29" t="s">
+        <v>275</v>
+      </c>
+      <c r="AD29" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>57</v>
+      </c>
+      <c r="B30" t="n" s="2">
+        <v>45300.3440162037</v>
+      </c>
+      <c r="C30" t="n" s="2">
+        <v>45309.346087962964</v>
+      </c>
+      <c r="D30" t="s">
+        <v>64</v>
+      </c>
+      <c r="E30" t="s">
+        <v>93</v>
+      </c>
+      <c r="F30" t="n">
+        <v>77.0</v>
+      </c>
+      <c r="G30" t="n">
+        <v>777779.0</v>
+      </c>
+      <c r="H30" t="s">
+        <v>101</v>
+      </c>
+      <c r="I30" t="n" s="2">
+        <v>45313.31128472222</v>
+      </c>
+      <c r="J30" t="s">
+        <v>130</v>
+      </c>
+      <c r="K30" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L30" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="M30" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="N30" t="s">
+        <v>137</v>
+      </c>
+      <c r="O30" t="s">
+        <v>138</v>
+      </c>
+      <c r="P30" t="s">
+        <v>139</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>141</v>
+      </c>
+      <c r="R30" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="S30" t="s">
+        <v>148</v>
+      </c>
+      <c r="T30" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="U30" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="V30" t="s">
+        <v>151</v>
+      </c>
+      <c r="W30" t="s">
+        <v>140</v>
+      </c>
+      <c r="X30" t="s">
+        <v>140</v>
+      </c>
+      <c r="Y30" t="s">
+        <v>183</v>
+      </c>
+      <c r="Z30" t="s">
+        <v>214</v>
+      </c>
+      <c r="AA30" t="s">
+        <v>218</v>
+      </c>
+      <c r="AB30" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AC30" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AD30" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>58</v>
+      </c>
+      <c r="B31" t="n" s="2">
+        <v>45310.76914351852</v>
+      </c>
+      <c r="C31" t="n" s="2">
+        <v>45310.77340277778</v>
+      </c>
+      <c r="D31" t="s">
+        <v>64</v>
+      </c>
+      <c r="E31" t="s">
+        <v>94</v>
+      </c>
+      <c r="F31" t="n">
+        <v>54.0</v>
+      </c>
+      <c r="G31" t="n">
+        <v>368.0</v>
+      </c>
+      <c r="H31" t="s">
+        <v>101</v>
+      </c>
+      <c r="I31" t="n" s="2">
+        <v>45313.31128472222</v>
+      </c>
+      <c r="J31" t="s">
+        <v>131</v>
+      </c>
+      <c r="K31" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L31" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="M31" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="N31" t="s">
+        <v>137</v>
+      </c>
+      <c r="O31" t="s">
+        <v>138</v>
+      </c>
+      <c r="P31" t="s">
+        <v>139</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>142</v>
+      </c>
+      <c r="R31" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="S31" t="s">
+        <v>148</v>
+      </c>
+      <c r="T31" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="U31" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="V31" t="s">
+        <v>155</v>
+      </c>
+      <c r="W31" t="s">
+        <v>139</v>
+      </c>
+      <c r="X31" t="s">
+        <v>139</v>
+      </c>
+      <c r="Y31" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="Z31" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AA31"/>
+      <c r="AB31" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AC31" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AD31" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>59</v>
+      </c>
+      <c r="B32" t="n" s="2">
+        <v>45238.622037037036</v>
+      </c>
+      <c r="C32" t="n" s="2">
+        <v>45244.57711805556</v>
+      </c>
+      <c r="D32" t="s">
+        <v>64</v>
+      </c>
+      <c r="E32" t="s">
+        <v>95</v>
+      </c>
+      <c r="F32" t="n">
+        <v>77.0</v>
+      </c>
+      <c r="G32" t="n">
+        <v>514519.0</v>
+      </c>
+      <c r="H32" t="s">
+        <v>101</v>
+      </c>
+      <c r="I32" t="n" s="2">
+        <v>45313.31129629629</v>
+      </c>
+      <c r="J32" t="s">
+        <v>132</v>
+      </c>
+      <c r="K32" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L32" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="M32" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="N32" t="s">
+        <v>137</v>
+      </c>
+      <c r="O32" t="s">
+        <v>138</v>
+      </c>
+      <c r="P32" t="s">
+        <v>139</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>144</v>
+      </c>
+      <c r="R32" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="S32" t="s">
+        <v>148</v>
+      </c>
+      <c r="T32" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="U32" t="n">
+        <v>25.0</v>
+      </c>
+      <c r="V32" t="s">
+        <v>151</v>
+      </c>
+      <c r="W32" t="s">
+        <v>140</v>
+      </c>
+      <c r="X32" t="s">
+        <v>140</v>
+      </c>
+      <c r="Y32" t="s">
+        <v>184</v>
+      </c>
+      <c r="Z32" t="s">
+        <v>215</v>
+      </c>
+      <c r="AA32" t="s">
+        <v>218</v>
+      </c>
+      <c r="AB32" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AC32" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AD32" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>60</v>
+      </c>
+      <c r="B33" t="n" s="2">
+        <v>45299.554560185185</v>
+      </c>
+      <c r="C33" t="n" s="2">
+        <v>45299.569340277776</v>
+      </c>
+      <c r="D33" t="s">
+        <v>64</v>
+      </c>
+      <c r="E33" t="s">
+        <v>96</v>
+      </c>
+      <c r="F33" t="n">
+        <v>77.0</v>
+      </c>
+      <c r="G33" t="n">
+        <v>1277.0</v>
+      </c>
+      <c r="H33" t="s">
+        <v>101</v>
+      </c>
+      <c r="I33" t="n" s="2">
+        <v>45313.31135416667</v>
+      </c>
+      <c r="J33" t="s">
+        <v>133</v>
+      </c>
+      <c r="K33" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L33" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="M33" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="N33" t="s">
+        <v>137</v>
+      </c>
+      <c r="O33" t="s">
+        <v>138</v>
+      </c>
+      <c r="P33" t="s">
+        <v>139</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>143</v>
+      </c>
+      <c r="R33" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="S33" t="s">
+        <v>150</v>
+      </c>
+      <c r="T33" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="U33" t="n">
+        <v>33.0</v>
+      </c>
+      <c r="V33" t="s">
+        <v>151</v>
+      </c>
+      <c r="W33" t="s">
+        <v>139</v>
+      </c>
+      <c r="X33" t="s">
+        <v>139</v>
+      </c>
+      <c r="Y33" t="s">
         <v>185</v>
       </c>
-      <c r="AA29" t="s">
+      <c r="Z33" t="s">
+        <v>216</v>
+      </c>
+      <c r="AA33" t="s">
+        <v>220</v>
+      </c>
+      <c r="AB33" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AC33" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AD33" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>61</v>
+      </c>
+      <c r="B34" t="n" s="2">
+        <v>45302.56277777778</v>
+      </c>
+      <c r="C34" t="n" s="2">
+        <v>45306.60188657408</v>
+      </c>
+      <c r="D34" t="s">
+        <v>64</v>
+      </c>
+      <c r="E34" t="s">
+        <v>97</v>
+      </c>
+      <c r="F34" t="n">
+        <v>54.0</v>
+      </c>
+      <c r="G34" t="n">
+        <v>348979.0</v>
+      </c>
+      <c r="H34" t="s">
+        <v>101</v>
+      </c>
+      <c r="I34" t="n" s="2">
+        <v>45313.31135416667</v>
+      </c>
+      <c r="J34" t="s">
+        <v>134</v>
+      </c>
+      <c r="K34" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L34" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="M34" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="N34" t="s">
+        <v>137</v>
+      </c>
+      <c r="O34" t="s">
+        <v>138</v>
+      </c>
+      <c r="P34" t="s">
+        <v>139</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>145</v>
+      </c>
+      <c r="R34" t="s">
+        <v>147</v>
+      </c>
+      <c r="S34" t="s">
+        <v>148</v>
+      </c>
+      <c r="T34" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="U34" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="V34" t="s">
+        <v>151</v>
+      </c>
+      <c r="W34" t="s">
+        <v>139</v>
+      </c>
+      <c r="X34" t="s">
+        <v>139</v>
+      </c>
+      <c r="Y34" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="Z34" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AA34"/>
+      <c r="AB34" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AC34" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AD34" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>62</v>
+      </c>
+      <c r="B35" t="n" s="2">
+        <v>45307.61559027778</v>
+      </c>
+      <c r="C35" t="n" s="2">
+        <v>45307.61708333333</v>
+      </c>
+      <c r="D35" t="s">
+        <v>64</v>
+      </c>
+      <c r="E35" t="s">
+        <v>98</v>
+      </c>
+      <c r="F35" t="n">
+        <v>54.0</v>
+      </c>
+      <c r="G35" t="n">
+        <v>128.0</v>
+      </c>
+      <c r="H35" t="s">
+        <v>101</v>
+      </c>
+      <c r="I35" t="n" s="2">
+        <v>45313.31135416667</v>
+      </c>
+      <c r="J35" t="s">
+        <v>135</v>
+      </c>
+      <c r="K35" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L35" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="M35" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="N35" t="s">
+        <v>137</v>
+      </c>
+      <c r="O35" t="s">
+        <v>138</v>
+      </c>
+      <c r="P35" t="s">
+        <v>139</v>
+      </c>
+      <c r="Q35" t="s">
+        <v>142</v>
+      </c>
+      <c r="R35" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="S35" t="s">
+        <v>148</v>
+      </c>
+      <c r="T35" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="U35" t="n">
+        <v>23.0</v>
+      </c>
+      <c r="V35" t="s">
+        <v>151</v>
+      </c>
+      <c r="W35" t="s">
+        <v>139</v>
+      </c>
+      <c r="X35" t="s">
+        <v>140</v>
+      </c>
+      <c r="Y35" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="Z35" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AA35"/>
+      <c r="AB35" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AC35" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AD35" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>63</v>
+      </c>
+      <c r="B36" t="n" s="2">
+        <v>45306.501875</v>
+      </c>
+      <c r="C36" t="n" s="2">
+        <v>45306.50971064815</v>
+      </c>
+      <c r="D36" t="s">
+        <v>64</v>
+      </c>
+      <c r="E36" t="s">
+        <v>99</v>
+      </c>
+      <c r="F36" t="n">
+        <v>77.0</v>
+      </c>
+      <c r="G36" t="n">
+        <v>677.0</v>
+      </c>
+      <c r="H36" t="s">
+        <v>101</v>
+      </c>
+      <c r="I36" t="n" s="2">
+        <v>45313.31135416667</v>
+      </c>
+      <c r="J36" t="s">
+        <v>136</v>
+      </c>
+      <c r="K36" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L36" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="M36" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="N36" t="s">
+        <v>137</v>
+      </c>
+      <c r="O36" t="s">
+        <v>138</v>
+      </c>
+      <c r="P36" t="s">
+        <v>139</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>143</v>
+      </c>
+      <c r="R36" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="S36" t="s">
+        <v>150</v>
+      </c>
+      <c r="T36" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="U36" t="n">
+        <v>25.0</v>
+      </c>
+      <c r="V36" t="s">
+        <v>151</v>
+      </c>
+      <c r="W36" t="s">
+        <v>139</v>
+      </c>
+      <c r="X36" t="s">
+        <v>139</v>
+      </c>
+      <c r="Y36" t="s">
         <v>186</v>
       </c>
-      <c r="AB29" t="s">
-        <v>216</v>
-      </c>
-      <c r="AC29" t="s">
-        <v>243</v>
-      </c>
-      <c r="AD29" t="s">
-        <v>270</v>
+      <c r="Z36" t="s">
+        <v>217</v>
+      </c>
+      <c r="AA36" t="s">
+        <v>218</v>
+      </c>
+      <c r="AB36" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AC36" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AD36" t="e">
+        <v>#N/A</v>
       </c>
     </row>
   </sheetData>

</xml_diff>